<commit_message>
Links added in Govt scheme
</commit_message>
<xml_diff>
--- a/govt aided schemes/govt_schemes.xlsx
+++ b/govt aided schemes/govt_schemes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirti\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41c4ab87885fd82d/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9930B82C-E44F-4A35-BBE2-1E42909DA739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="14_{33830C7A-9471-4095-8464-0F557495317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BAE35B-D938-4F57-9D77-D593BCF201CA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD2C649B-7986-471F-8B6F-2885A4982D96}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>All India</t>
   </si>
@@ -241,15 +241,71 @@
   <si>
     <t>Eligibilty_criteria</t>
   </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>https://pmfby.gov.in/</t>
+  </si>
+  <si>
+    <t>https://pmksy.gov.in/</t>
+  </si>
+  <si>
+    <t>https://jalshakti-ddws.gov.in/</t>
+  </si>
+  <si>
+    <t>https://soilhealth.dac.gov.in/</t>
+  </si>
+  <si>
+    <t>http://agricoop.gov.in/</t>
+  </si>
+  <si>
+    <t>https://pmkisan.gov.in/</t>
+  </si>
+  <si>
+    <t>https://agricoop.nic.in/</t>
+  </si>
+  <si>
+    <t>https://www.enam.gov.in/web/</t>
+  </si>
+  <si>
+    <t>https://www.kalia.co.in/</t>
+  </si>
+  <si>
+    <t>https://odishaeiz.gov.in/</t>
+  </si>
+  <si>
+    <t>http://agriodisha.nic.in/</t>
+  </si>
+  <si>
+    <t>http://www.dowrorissa.gov.in/</t>
+  </si>
+  <si>
+    <t>http://agriodisha.nic.in/schemes/odisha-millets-mission/</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>https://upagriculture.com/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,10 +328,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -283,8 +340,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -597,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EB68AB-D548-4777-AFB4-3B1C26B4199A}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="47" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="70" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,9 +670,10 @@
     <col min="2" max="2" width="37.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.21875" style="2" customWidth="1"/>
     <col min="4" max="4" width="39.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -623,8 +686,11 @@
       <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -637,8 +703,11 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -651,8 +720,11 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -665,8 +737,11 @@
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E4" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -679,8 +754,11 @@
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -693,8 +771,11 @@
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="E6" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -707,8 +788,11 @@
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="E7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -721,8 +805,11 @@
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="E8" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -735,8 +822,11 @@
       <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="288" x14ac:dyDescent="0.3">
+      <c r="E9" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="288" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -749,8 +839,11 @@
       <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="E10" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -763,8 +856,11 @@
       <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -777,8 +873,11 @@
       <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="E12" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -791,8 +890,11 @@
       <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="E13" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -807,8 +909,12 @@
         <f>D2</f>
         <v>The scheme is applicable to all food and oilseed crops, horticultural crops, and commercial and annual crops. Farmers can enroll for the scheme for any of the notified crops in their area. However, the scheme is voluntary, and farmers can choose whether or not to enroll.</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E14" s="2" t="str">
+        <f>E2</f>
+        <v>https://pmfby.gov.in/</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -823,8 +929,12 @@
         <f>D3</f>
         <v xml:space="preserve"> Available to all farmers in India who are dependent on irrigation for their crops, as well as to other stakeholders involved in the irrigation supply chain. The scheme is primarily implemented by state governments, and interested farmers and stakeholders can contact the State Irrigation Department or the concerned nodal agency in their state to apply for the scheme.</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="str">
+        <f>E3</f>
+        <v>https://jalshakti-ddws.gov.in/</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -837,8 +947,11 @@
       <c r="D16" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="E16" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -853,8 +966,12 @@
         <f>D6</f>
         <v>all farmers in India, including small and marginal farmers, sharecroppers, oral lessees, and tenant farmers, are eligible to apply for the Kisan Credit Card scheme. The scheme aims to provide farmers with access to affordable credit for their agricultural activities, and the application process is simple and easy to follow.</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E17" s="2" t="str">
+        <f>E6</f>
+        <v>https://pmkisan.gov.in/</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -869,8 +986,11 @@
         <f>D4</f>
         <v>all farmers in India can apply for the Soil Health Card Scheme. The scheme is implemented through a network of soil testing labs, and farmers can apply by contacting their nearest agriculture department office or visiting the website of the Department of Agriculture and Cooperation.</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -885,8 +1005,12 @@
         <f>D8</f>
         <v>all farmers, traders, and buyers with a valid PAN card, Aadhaar card, and bank account can apply to use the National Agriculture Market (eNAM) platform. The eNAM platform aims to provide farmers with an opportunity to sell their produce beyond their local markets and get better prices for their produce, while also providing traders and buyers with access to a larger number of sellers and an efficient way to purchase agricultural produce.</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="E19" s="2" t="str">
+        <f>E8</f>
+        <v>https://www.enam.gov.in/web/</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -895,20 +1019,24 @@
         <v>Pradhan Mantri Fasal Bima Yojana (PMFBY)</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f t="shared" ref="C20:D20" si="0">C14</f>
+        <f t="shared" ref="C20:E20" si="0">C14</f>
         <v xml:space="preserve"> This is an insurance scheme for farmers that provides financial assistance in case of crop loss due to natural calamities. Under the PMFBY scheme, farmers pay a premium of 2% of the sum insured for Kharif crops, 1.5% for Rabi crops, and 5% for annual commercial and horticultural crops. The remaining premium is paid by the government. The sum insured is fixed based on the scale of finance for each crop.</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>The scheme is applicable to all food and oilseed crops, horticultural crops, and commercial and annual crops. Farmers can enroll for the scheme for any of the notified crops in their area. However, the scheme is voluntary, and farmers can choose whether or not to enroll.</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://pmfby.gov.in/</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f t="shared" ref="B21:D21" si="1">B15</f>
+        <f t="shared" ref="B21:E21" si="1">B15</f>
         <v>Pradhan Mantri Krishi Sinchai Yojana (PMKSY)</v>
       </c>
       <c r="C21" s="2" t="str">
@@ -919,13 +1047,17 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> Available to all farmers in India who are dependent on irrigation for their crops, as well as to other stakeholders involved in the irrigation supply chain. The scheme is primarily implemented by state governments, and interested farmers and stakeholders can contact the State Irrigation Department or the concerned nodal agency in their state to apply for the scheme.</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="E21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://jalshakti-ddws.gov.in/</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f t="shared" ref="B22:D22" si="2">B16</f>
+        <f t="shared" ref="B22:E22" si="2">B16</f>
         <v>Pradhan Mantri Krishi Sampada Yojana (PMKSY)</v>
       </c>
       <c r="C22" s="2" t="str">
@@ -942,13 +1074,17 @@
 The applicant should have the necessary infrastructure and facilities to undertake food processing activities.
 The applicant should have a good track record and financial history, and should not have defaulted on any previous loans or government schemes.</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="E22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://pmksy.gov.in/</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f t="shared" ref="B23:D23" si="3">B17</f>
+        <f t="shared" ref="B23:E23" si="3">B17</f>
         <v>Kisan Credit Card Scheme</v>
       </c>
       <c r="C23" s="2" t="str">
@@ -959,13 +1095,17 @@
         <f t="shared" si="3"/>
         <v>all farmers in India, including small and marginal farmers, sharecroppers, oral lessees, and tenant farmers, are eligible to apply for the Kisan Credit Card scheme. The scheme aims to provide farmers with access to affordable credit for their agricultural activities, and the application process is simple and easy to follow.</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E23" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://pmkisan.gov.in/</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f t="shared" ref="B24:D24" si="4">B18</f>
+        <f t="shared" ref="B24:E24" si="4">B18</f>
         <v>Soil Health Card Scheme</v>
       </c>
       <c r="C24" s="2" t="str">
@@ -976,8 +1116,15 @@
         <f t="shared" si="4"/>
         <v>all farmers in India can apply for the Soil Health Card Scheme. The scheme is implemented through a network of soil testing labs, and farmers can apply by contacting their nearest agriculture department office or visiting the website of the Department of Agriculture and Cooperation.</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="288" x14ac:dyDescent="0.3">
+      <c r="E24" s="2" t="str">
+        <f>E18</f>
+        <v>https://soilhealth.dac.gov.in/</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
@@ -987,10 +1134,30 @@
       <c r="D25" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="E25" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{818372BD-D799-4901-AF21-7C890863C7BB}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{64B3AAC5-AF5F-48CF-8EAA-7246389DA4F6}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{54407720-E803-4717-BDAD-C8B4646AF782}"/>
+    <hyperlink ref="E18" r:id="rId4" xr:uid="{331FA344-C567-4F1F-AF0D-2904F39F698F}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{05F6D683-849E-4545-82D8-55034B3F5DE9}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{02F13840-CA3F-428B-8D57-66BEFEAB62AB}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{158ADEDE-1863-4D0B-BDEB-C8985ECD762B}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{8BC1C9B4-9ED5-4BEE-A929-C0AD51066298}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{5100C9D2-4CD4-48E6-9F52-BED926A78D56}"/>
+    <hyperlink ref="E10" r:id="rId10" xr:uid="{D31C492F-C405-48D3-9EF8-77384B90F6EF}"/>
+    <hyperlink ref="E11" r:id="rId11" xr:uid="{B4A60897-2D86-4589-A90F-5D203CDF7E69}"/>
+    <hyperlink ref="E12" r:id="rId12" xr:uid="{8F6A7081-D83F-4C3B-9231-2465FB80D5E8}"/>
+    <hyperlink ref="E13" r:id="rId13" xr:uid="{A3ADD624-1CB0-4727-894E-8B114EDCF38C}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{8008E7F6-BACF-41AB-8AAC-7861CE2CA4CF}"/>
+    <hyperlink ref="E25" r:id="rId15" xr:uid="{FC427ECB-0B9F-4C3E-B574-1CFCE8AB492F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">

</xml_diff>

<commit_message>
More states are added in govt_scheme
</commit_message>
<xml_diff>
--- a/govt aided schemes/govt_schemes.xlsx
+++ b/govt aided schemes/govt_schemes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41c4ab87885fd82d/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41c4ab87885fd82d/Desktop/AgroInOne/govt aided schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="14_{33830C7A-9471-4095-8464-0F557495317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BAE35B-D938-4F57-9D77-D593BCF201CA}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="14_{33830C7A-9471-4095-8464-0F557495317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7DCD84D-BCEF-4219-8D8C-A2919926DE8B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD2C649B-7986-471F-8B6F-2885A4982D96}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
   <si>
     <t>All India</t>
   </si>
@@ -193,9 +193,6 @@
 The applicant should not have availed any other subsidy or benefits for the same crop under any other scheme.</t>
   </si>
   <si>
-    <t>Punjab</t>
-  </si>
-  <si>
     <t>Pradhan Mantri Krishi Sampada Yojana (PMKSY)</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
 The project should adhere to all relevant regulations and guidelines related to food safety, quality, and standards.
 The applicant should have the necessary infrastructure and facilities to undertake food processing activities.
 The applicant should have a good track record and financial history, and should not have defaulted on any previous loans or government schemes.</t>
-  </si>
-  <si>
-    <t>Haryana</t>
   </si>
   <si>
     <t>Mukhyamantri Kisan Khet Sadak Yojana (MKKSY)</t>
@@ -269,32 +263,211 @@
     <t>https://www.enam.gov.in/web/</t>
   </si>
   <si>
-    <t>https://www.kalia.co.in/</t>
-  </si>
-  <si>
     <t>https://odishaeiz.gov.in/</t>
   </si>
   <si>
-    <t>http://agriodisha.nic.in/</t>
-  </si>
-  <si>
-    <t>http://www.dowrorissa.gov.in/</t>
-  </si>
-  <si>
-    <t>http://agriodisha.nic.in/schemes/odisha-millets-mission/</t>
-  </si>
-  <si>
     <t>UP</t>
   </si>
   <si>
-    <t>https://upagriculture.com/</t>
+    <t>Punjab/Haryana</t>
+  </si>
+  <si>
+    <t>http://upagriculture.com/</t>
+  </si>
+  <si>
+    <t>https://kaliaportal.odisha.gov.in/TrackToken.aspx</t>
+  </si>
+  <si>
+    <t>https://agri.odisha.gov.in/schemes-agriculture/agriculture</t>
+  </si>
+  <si>
+    <t>http://www.dowrodisha.gov.in/</t>
+  </si>
+  <si>
+    <t>https://milletsodisha.com/</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh Kisan Rin Mochan Yojana</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh Mukhyamantri Kisan Ayam Sarvhit Bima Yojana</t>
+  </si>
+  <si>
+    <t>The Uttar Pradesh Mukhyamantri Kisan Ayam Sarvhit Bima Yojana is an insurance scheme launched by the Government of Uttar Pradesh to provide insurance coverage to farmers and their families in case of death or disability due to accidents. The objective of the scheme is to provide social security to farmers and their families.</t>
+  </si>
+  <si>
+    <t>The farmer should be a resident of Uttar Pradesh.
+The farmer should be between the ages of 18 and 70 years.
+The farmer should be engaged in agricultural activities.
+The farmer should have a valid Aadhaar card.
+The farmer's family members, including the spouse and dependent children, are eligible for the insurance coverage.
+The farmer should not have any criminal record.</t>
+  </si>
+  <si>
+    <t>https://upagripardarshi.gov.in/</t>
+  </si>
+  <si>
+    <t>It is a debt waiver scheme launched by the Government of Uttar Pradesh to waive off the loans of small and marginal farmers in the state. The objective of the scheme is to provide financial relief to farmers who are unable to repay their agricultural loans due to various reasons, including crop failure, natural calamities, and other unforeseen events.</t>
+  </si>
+  <si>
+    <t>The farmer should be a resident of Uttar Pradesh.
+The farmer should have taken a loan from any scheduled commercial bank, cooperative bank, or regional rural bank.
+The loan should be classified as non-performing asset (NPA) or overdue as of 31st March 2016.
+The loan amount should not exceed Rs. 1 lakh.
+The farmer's landholding should be less than 2 hectares.</t>
+  </si>
+  <si>
+    <t>https://upcane.gov.in/</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Subhiksha Keralam is an ambitious project launched by the Government of Kerala aimed at making the state self-sufficient in food production. The scheme covers various aspects of agriculture such as cultivation, animal husbandry, fisheries, and agro-processing. It offers various incentives and subsidies to farmers to encourage them to adopt modern farming practices.</t>
+  </si>
+  <si>
+    <t>State Plan Schemes</t>
+  </si>
+  <si>
+    <t>Kerala State Plan Schemes provide various incentives and subsidies to farmers for promoting agriculture and allied sectors. The schemes cover activities such as land development, irrigation, farm mechanization, seed production, and livestock development.</t>
+  </si>
+  <si>
+    <t>Kerala Agriculture Farmers Welfare Fund Act, 2018</t>
+  </si>
+  <si>
+    <t>The Kerala Agriculture Farmers Welfare Fund Act, 2018, is a state government scheme aimed at providing financial support to farmers in case of crop loss or damage due to natural calamities. Under this scheme, farmers are entitled to compensation based on the extent of crop loss or damage.</t>
+  </si>
+  <si>
+    <t>Farmers who have agricultural land can participate in this scheme.
+Preference is given to farmers who have taken land on lease for a minimum of three years.
+The age limit of the farmers should be between 18 to 60 years.</t>
+  </si>
+  <si>
+    <t>Subhiksha Keralam Vegetable Cultivation Program</t>
+  </si>
+  <si>
+    <t>Subhiksha Keralam Dairy Farming Program</t>
+  </si>
+  <si>
+    <t>Subhiksha Keralam Paddy Cultivation Program</t>
+  </si>
+  <si>
+    <t>Farmers who own indigenous cows or buffaloes can participate in this scheme.
+Farmers who do not have cows or buffaloes can avail of bank loans to purchase them.
+The age limit of the farmers should be between 18 to 60 years.</t>
+  </si>
+  <si>
+    <t>https://keralaagriculture.gov.in/en/10951-2/</t>
+  </si>
+  <si>
+    <t>Residence: The applicant must be a resident of the state for which the scheme is being implemented.
+Age: The minimum and maximum age limit of the applicant may vary depending on the scheme. In general, the age limit should be between 18 to 60 years.
+Income: The income limit of the applicant may vary depending on the scheme. Some schemes may have a specific income limit, while others may not have any income limit.
+Education: The educational qualification of the applicant may vary depending on the scheme. Some schemes may require a minimum educational qualification, while others may not have any such requirement.
+Social Category: Some schemes may be targeted towards specific social categories such as Scheduled Castes, Scheduled Tribes, Other Backward Classes, etc. In such cases, the applicant must belong to the specific social category.</t>
+  </si>
+  <si>
+    <t>https://cooperation.kerala.gov.in/category/schemes/state-plan-schemes/</t>
+  </si>
+  <si>
+    <t>Resident of Kerala: The applicant must be a resident of Kerala.
+Farmer: The applicant must be a farmer engaged in agriculture or allied activities, including crop cultivation, animal husbandry, fisheries, and forestry.
+Landholding: The applicant must have a landholding in Kerala.
+Bank account: The applicant must have a bank account in his/her name.
+Identification: The applicant must possess a valid identification document such as an Aadhaar card or Voter ID.</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Tamil Nadu State Agricultural Marketing Board Scheme</t>
+  </si>
+  <si>
+    <t>The applicant must be a resident of Tamil Nadu.
+The applicant must be engaged in seed production, processing, or marketing activities.
+The applicant must have a valid identification document such as an Aadhaar card or Voter ID.</t>
+  </si>
+  <si>
+    <t>https://seedcertification.tn.gov.in/seed/login/login.php</t>
+  </si>
+  <si>
+    <t>The Tamil Nadu State Agricultural Marketing Board implements various schemes for the welfare of farmers and the development of agricultural marketing in the state. Some of the schemes include:
+Construction of new regulated markets
+Renovation and modernization of existing regulated markets
+Provision of infrastructure facilities like auction platforms, cold storages, grading and sorting units, etc.
+Promotion of direct marketing by farmers
+Development of value chains for agricultural commodities</t>
+  </si>
+  <si>
+    <t>Tamil Nadu Agricultural Insurance Scheme</t>
+  </si>
+  <si>
+    <t>The applicant must be a resident of Tamil Nadu.
+The applicant must be engaged in agricultural activities, including crop cultivation, animal husbandry, fisheries, and forestry.
+The applicant must have a valid identification document such as an Aadhaar card or Voter ID.</t>
+  </si>
+  <si>
+    <t>Tamil Nadu Agricultural Marketing and Agri Business Department Scheme</t>
+  </si>
+  <si>
+    <t>The applicant must be a resident of Tamil Nadu.
+The applicant must be engaged in agriculture or allied activities, including crop cultivation, animal husbandry, fisheries, and forestry.
+The applicant must have a valid identification document such as an Aadhaar card or Voter ID.</t>
+  </si>
+  <si>
+    <t>Tamil Nadu Horticulture Development Agency Scheme</t>
+  </si>
+  <si>
+    <t>The applicant must be a resident of Tamil Nadu.
+The applicant must be engaged in horticulture activities, including fruit and vegetable cultivation, floriculture, medicinal and aromatic plants, etc.
+The applicant must have a valid identification document such as an Aadhaar card or Voter ID.</t>
+  </si>
+  <si>
+    <t>Tamil Nadu Agricultural University Scheme</t>
+  </si>
+  <si>
+    <t>The applicant must be a resident of Tamil Nadu.
+The applicant must be interested in pursuing higher education in agriculture or allied subjects.
+The applicant must have completed the required educational qualifications and have a valid identification document such as an Aadhaar card or Voter ID.</t>
+  </si>
+  <si>
+    <t>Tamil Nadu Agricultural Insurance Scheme (TNAIS) is a state-sponsored crop insurance scheme aimed at providing financial support to farmers in case of crop loss due to natural calamities, pests, and diseases. The scheme is implemented by the Tamil Nadu Agricultural Insurance and Risk Management Corporation (TNAIS) and covers all farmers in the state who own up to 2 hectares of land.</t>
+  </si>
+  <si>
+    <t>https://www.tn.gov.in/scheme/data_view/66633</t>
+  </si>
+  <si>
+    <t>Tamil Nadu Agricultural Marketing and Agri Business Department implements various schemes to promote agriculture and allied activities in the state. Some of the important schemes are:                                Tamil Nadu Agri Business and Rural Transformation Project (TANUVAS-TNABARD-NABARD)             Integrated Scheme for Agricultural Marketing (ISAM)                                                                                                   Tamil Nadu State Agricultural Marketing Board (TNSAMB</t>
+  </si>
+  <si>
+    <t>https://www.agrimark.tn.gov.in/</t>
+  </si>
+  <si>
+    <t>The Tamil Nadu Horticulture Development Agency (TANHODA) has several schemes for the development of horticulture in the state. Some of the schemes are                                                                                                    Integrated Horticulture Development Scheme
+Micro Irrigation Scheme
+National Horticulture Mission
+Horticulture Technology Mission
+Agriculture Technology Management Agency</t>
+  </si>
+  <si>
+    <t>https://tnhorticulture.tn.gov.in/</t>
+  </si>
+  <si>
+    <t>The Tamil Nadu Agricultural University (TNAU) offers various schemes to promote agriculture and allied fields in the state of Tamil Nadu, India. Some of the notable schemes include:
+Krishi Vigyan Kendra Scheme
+Integrated Farming System Scheme
+Precision Farming Development Centre Scheme
+Agri-Business Incubation Programme</t>
+  </si>
+  <si>
+    <t>https://tnau.ac.in/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +482,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -332,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -344,6 +523,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -659,35 +839,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EB68AB-D548-4777-AFB4-3B1C26B4199A}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="70" zoomScaleNormal="47" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="83" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="47.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="88.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="74.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="38.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
@@ -704,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
@@ -721,10 +902,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -738,7 +919,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
@@ -755,7 +936,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
@@ -772,7 +953,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
@@ -789,7 +970,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
@@ -806,10 +987,10 @@
         <v>21</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -823,10 +1004,10 @@
         <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -840,10 +1021,10 @@
         <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="374.4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="288" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -857,10 +1038,10 @@
         <v>35</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="288" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -874,10 +1055,10 @@
         <v>36</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="288" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -891,69 +1072,67 @@
         <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="str">
-        <f>C2</f>
+        <f t="shared" ref="C14:C15" si="0">C2</f>
         <v xml:space="preserve"> This is an insurance scheme for farmers that provides financial assistance in case of crop loss due to natural calamities. Under the PMFBY scheme, farmers pay a premium of 2% of the sum insured for Kharif crops, 1.5% for Rabi crops, and 5% for annual commercial and horticultural crops. The remaining premium is paid by the government. The sum insured is fixed based on the scale of finance for each crop.</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>D2</f>
         <v>The scheme is applicable to all food and oilseed crops, horticultural crops, and commercial and annual crops. Farmers can enroll for the scheme for any of the notified crops in their area. However, the scheme is voluntary, and farmers can choose whether or not to enroll.</v>
       </c>
-      <c r="E14" s="2" t="str">
-        <f>E2</f>
-        <v>https://pmfby.gov.in/</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="E14" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="str">
-        <f>C3</f>
+        <f t="shared" si="0"/>
         <v>This scheme aims to enhance the productivity of crops by providing water to farmers for irrigation purposes. The PMKSY scheme focuses on the development of water resources for agricultural purposes, and it has four components.</v>
       </c>
       <c r="D15" s="2" t="str">
         <f>D3</f>
         <v xml:space="preserve"> Available to all farmers in India who are dependent on irrigation for their crops, as well as to other stakeholders involved in the irrigation supply chain. The scheme is primarily implemented by state governments, and interested farmers and stakeholders can contact the State Irrigation Department or the concerned nodal agency in their state to apply for the scheme.</v>
       </c>
-      <c r="E15" s="2" t="str">
-        <f>E3</f>
-        <v>https://jalshakti-ddws.gov.in/</v>
+      <c r="E15" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>13</v>
@@ -966,14 +1145,13 @@
         <f>D6</f>
         <v>all farmers in India, including small and marginal farmers, sharecroppers, oral lessees, and tenant farmers, are eligible to apply for the Kisan Credit Card scheme. The scheme aims to provide farmers with access to affordable credit for their agricultural activities, and the application process is simple and easy to follow.</v>
       </c>
-      <c r="E17" s="2" t="str">
-        <f>E6</f>
-        <v>https://pmkisan.gov.in/</v>
+      <c r="E17" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
@@ -987,12 +1165,12 @@
         <v>all farmers in India can apply for the Soil Health Card Scheme. The scheme is implemented through a network of soil testing labs, and farmers can apply by contacting their nearest agriculture department office or visiting the website of the Department of Agriculture and Cooperation.</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>
@@ -1005,137 +1183,229 @@
         <f>D8</f>
         <v>all farmers, traders, and buyers with a valid PAN card, Aadhaar card, and bank account can apply to use the National Agriculture Market (eNAM) platform. The eNAM platform aims to provide farmers with an opportunity to sell their produce beyond their local markets and get better prices for their produce, while also providing traders and buyers with access to a larger number of sellers and an efficient way to purchase agricultural produce.</v>
       </c>
-      <c r="E19" s="2" t="str">
-        <f>E8</f>
-        <v>https://www.enam.gov.in/web/</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="E19" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="288" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="2" t="str">
-        <f>B14</f>
-        <v>Pradhan Mantri Fasal Bima Yojana (PMFBY)</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f t="shared" ref="C20:E20" si="0">C14</f>
-        <v xml:space="preserve"> This is an insurance scheme for farmers that provides financial assistance in case of crop loss due to natural calamities. Under the PMFBY scheme, farmers pay a premium of 2% of the sum insured for Kharif crops, 1.5% for Rabi crops, and 5% for annual commercial and horticultural crops. The remaining premium is paid by the government. The sum insured is fixed based on the scale of finance for each crop.</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>The scheme is applicable to all food and oilseed crops, horticultural crops, and commercial and annual crops. Farmers can enroll for the scheme for any of the notified crops in their area. However, the scheme is voluntary, and farmers can choose whether or not to enroll.</v>
-      </c>
-      <c r="E20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://pmfby.gov.in/</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="2" t="str">
-        <f t="shared" ref="B21:E21" si="1">B15</f>
-        <v>Pradhan Mantri Krishi Sinchai Yojana (PMKSY)</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>This scheme aims to enhance the productivity of crops by providing water to farmers for irrigation purposes. The PMKSY scheme focuses on the development of water resources for agricultural purposes, and it has four components.</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> Available to all farmers in India who are dependent on irrigation for their crops, as well as to other stakeholders involved in the irrigation supply chain. The scheme is primarily implemented by state governments, and interested farmers and stakeholders can contact the State Irrigation Department or the concerned nodal agency in their state to apply for the scheme.</v>
-      </c>
-      <c r="E21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jalshakti-ddws.gov.in/</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="2" t="str">
-        <f t="shared" ref="B22:E22" si="2">B16</f>
-        <v>Pradhan Mantri Krishi Sampada Yojana (PMKSY)</v>
-      </c>
-      <c r="C22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>This scheme aims to promote food processing industries and create employment opportunities in rural areas. The scheme includes various components such as infrastructure development, value addition, and market linkage.</v>
-      </c>
-      <c r="D22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Farmers, individuals, groups of farmers, cooperatives, companies, NGOs, and other organizations involved in the agriculture and food processing sector can apply for the scheme.
-The scheme is open to all states and union territories in India.
-The applicant should have a valid business plan and project report for the proposed food processing project.
-The project should be technically and financially viable, and should have the potential to generate employment opportunities.
-The project should adhere to all relevant regulations and guidelines related to food safety, quality, and standards.
-The applicant should have the necessary infrastructure and facilities to undertake food processing activities.
-The applicant should have a good track record and financial history, and should not have defaulted on any previous loans or government schemes.</v>
-      </c>
-      <c r="E22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>https://pmksy.gov.in/</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="2" t="str">
-        <f t="shared" ref="B23:E23" si="3">B17</f>
-        <v>Kisan Credit Card Scheme</v>
-      </c>
-      <c r="C23" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>This scheme provides farmers with credit facilities to meet their agricultural needs. To apply for the Kisan Credit Card scheme, farmers can approach any bank branch or cooperative society that is authorized to issue KCCs. The application process is straightforward and involves submitting basic identity and address proofs, as well as land and crop-related documents, to the bank or cooperative society.</v>
-      </c>
-      <c r="D23" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>all farmers in India, including small and marginal farmers, sharecroppers, oral lessees, and tenant farmers, are eligible to apply for the Kisan Credit Card scheme. The scheme aims to provide farmers with access to affordable credit for their agricultural activities, and the application process is simple and easy to follow.</v>
-      </c>
-      <c r="E23" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>https://pmkisan.gov.in/</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="2" t="str">
-        <f t="shared" ref="B24:E24" si="4">B18</f>
-        <v>Soil Health Card Scheme</v>
-      </c>
-      <c r="C24" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>This scheme aims to provide soil health cards to farmers, which contain information about the soil quality and fertility of their land. Under the Soil Health Card Scheme, soil health cards are issued to farmers after their soil samples are tested in accredited soil testing labs. These cards contain information on the soil health status of the farmer's land and provide recommendations on the type and quantity of nutrients that need to be added to the soil to improve its fertility.</v>
-      </c>
-      <c r="D24" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>all farmers in India can apply for the Soil Health Card Scheme. The scheme is implemented through a network of soil testing labs, and farmers can apply by contacting their nearest agriculture department office or visiting the website of the Department of Agriculture and Cooperation.</v>
-      </c>
-      <c r="E24" s="2" t="str">
-        <f>E18</f>
-        <v>https://soilhealth.dac.gov.in/</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>65</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="159" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1154,10 +1424,26 @@
     <hyperlink ref="E12" r:id="rId12" xr:uid="{8F6A7081-D83F-4C3B-9231-2465FB80D5E8}"/>
     <hyperlink ref="E13" r:id="rId13" xr:uid="{A3ADD624-1CB0-4727-894E-8B114EDCF38C}"/>
     <hyperlink ref="E16" r:id="rId14" xr:uid="{8008E7F6-BACF-41AB-8AAC-7861CE2CA4CF}"/>
-    <hyperlink ref="E25" r:id="rId15" xr:uid="{FC427ECB-0B9F-4C3E-B574-1CFCE8AB492F}"/>
+    <hyperlink ref="E20" r:id="rId15" xr:uid="{F43651E4-0CC3-4001-810D-9C082F4C9632}"/>
+    <hyperlink ref="E19" r:id="rId16" xr:uid="{FD1A79FF-6DB7-4D20-92C7-5541DD438407}"/>
+    <hyperlink ref="E17" r:id="rId17" xr:uid="{4A3D437F-358D-4579-8F6D-3F462162D594}"/>
+    <hyperlink ref="E15" r:id="rId18" xr:uid="{6BF7C7A4-E050-48C1-B627-3A4D0B4C6240}"/>
+    <hyperlink ref="E14" r:id="rId19" xr:uid="{A57F73B1-3890-4741-9973-AF07D8056663}"/>
+    <hyperlink ref="E22" r:id="rId20" xr:uid="{3E0A141A-6185-4FEE-9130-031CFCB8574D}"/>
+    <hyperlink ref="E21" r:id="rId21" xr:uid="{13FEC308-3FEE-4F64-8C25-DD377A9940F2}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{5ADE6A9C-4FA4-4909-9CA2-17C2F75B2D00}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{E8C915F1-0355-4A17-8895-84649B972059}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{35E68B67-E237-488C-A55B-D3DC4A12491B}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{7CC2BEC3-07FC-49B4-9257-AC3BDA4268EA}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{C3293722-7135-4628-AEC7-834BC9DA0484}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{29154396-57DF-4FB6-8B0F-22A3FEC31C24}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{DCB256DF-C4A6-4B50-AF77-3D74C6C5A262}"/>
+    <hyperlink ref="E30" r:id="rId29" xr:uid="{EDF017E9-5491-48E4-BA18-5B4DAC15CA6E}"/>
+    <hyperlink ref="E31" r:id="rId30" xr:uid="{0E0D11CB-F34A-4675-BE68-9D32B6A2FF91}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{5C626202-B02A-458E-BC2E-CC2042515F3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">

</xml_diff>

<commit_message>
more 9 states are added
</commit_message>
<xml_diff>
--- a/govt aided schemes/govt_schemes.xlsx
+++ b/govt aided schemes/govt_schemes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41c4ab87885fd82d/Desktop/AgroInOne/govt aided schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="14_{33830C7A-9471-4095-8464-0F557495317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7DCD84D-BCEF-4219-8D8C-A2919926DE8B}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="14_{33830C7A-9471-4095-8464-0F557495317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F797D837-1117-4FCB-BB16-0799E7264E96}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD2C649B-7986-471F-8B6F-2885A4982D96}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="308">
   <si>
     <t>All India</t>
   </si>
@@ -462,12 +462,642 @@
   <si>
     <t>https://tnau.ac.in/</t>
   </si>
+  <si>
+    <t>Jharkhand</t>
+  </si>
+  <si>
+    <t>1.Mukhyamantri Krishi Ashirwad Yojna</t>
+  </si>
+  <si>
+    <t>Mukhya Mantri Krishi AashirwadYojna is an ambitious scheme of the state government aimed at improving the financial situation of farmers and provide them with timely investment support before the start of the Kharif season. Benefits Marginal and small farmers will be given Rs 5000 per acre per year (maximum up to 5 Acres) through Direct Benefit Transfer in their bank account.</t>
+  </si>
+  <si>
+    <t>All the small and marginal farmers of the state, who have arable land up to a maximum of 5 acres are eligible to apply under the scheme.</t>
+  </si>
+  <si>
+    <t>https://hazaribag.nic.in/hi/document-category/</t>
+  </si>
+  <si>
+    <t>2.Jharkhand Krishi Rin Mafi Yojana</t>
+  </si>
+  <si>
+    <t>Jharkhand Krishi Rin Mafi Yojana, launched by the Jharkhand state government on 1 February 2021 is an agriculture loan waiver scheme for the farmers of Jharkhand. Benefits Under the scheme, the state government will waive loans of farmers upto Rs. 50,000 per farmer.</t>
+  </si>
+  <si>
+    <t> Must be a permanent resident of Jharkhand state.  The small and marginal farmers who have taken the loan using the Kisan Credit Card  Must be a farmer who self-cultivates his / her land OR farmers who cultivate in leased land  Must be at-least 18 years of age.  Only 1 farmer per family is allowed for loan waiver  The loan must have been availed from banks before 31 March 2020. Documents needed for application  Aadhaar number.  Ration card  Kisan Credit Card (KCC)</t>
+  </si>
+  <si>
+    <t>झारखण्ड कृषि ऋण माफी योजना</t>
+  </si>
+  <si>
+    <t>3.Jharkhand Kisan Fasal Rahat Yojana</t>
+  </si>
+  <si>
+    <t>Jharkhand Kisan Fasal Rahat Yojana aims to provide security cover to Jharkhand farmers in case of crop damage due to natural calamity</t>
+  </si>
+  <si>
+    <t> Farmers must be residents of Jharkhand.  Should be Small and marginal farmers  Both land and landless  Implementation agency</t>
+  </si>
+  <si>
+    <t>झारखण्ड राज्य फसल राहत योजना</t>
+  </si>
+  <si>
+    <t>4. Samakit Birsa Gram Vika Yojana cum Krishak Pathshala.</t>
+  </si>
+  <si>
+    <t>points  Under this scheme, one agriculture farm in every district will be selected.  Will be provided with various state-of the art technologies and tools of modern –day farming for horticulture, livestock’s rearing and pisciculture apart from new irrigation techniques.  Through this scheme, the farmers will be provided training and will be empowered to increase their incomes.  An approximate budget of Rs.50 crore has been allotted for the scheme for the fiscal year of 2021-22.</t>
+  </si>
+  <si>
+    <t>Farmer must be from jharkhand</t>
+  </si>
+  <si>
+    <t>Jharkhand Samekit Birsa Gram Vikas Yojana (Krishak Pathshala) 2023 | झारखण्ड समेकित बिरसा ग्राम विकास योजना (कृषक पाठशाला) Details</t>
+  </si>
+  <si>
+    <t>5. Birsa Kisan Yojana (BKY)</t>
+  </si>
+  <si>
+    <t>Jharkhand Chief Minister Hemant Soren announces new scheme details Birsa Kisan Yojana. This is a unique project start by the government for the betterment of farmers. In this scheme state government will make a unique ID card with a barcode for every farmer of Jharkhand state. With the help of this unique ID card, farmers can take benefit of different government schemes without any middleman. This initiative will also decrease the number of frauds that are held with farmers.</t>
+  </si>
+  <si>
+    <t>Under Birsa Kisan Scheme, the government will generate a unique ID card. This card will be generated after the registration of the farmer.  Farmers who want to register for this scheme have to carry their Aadhaar card with them.  Only one bank account will be linked to one phone number that you want to register.  The facility of direct bank transfer (DBT) is available for one bank account.  Enrollment of farmers will be held in Pragya Kendra. In enrollment, the farmer can do their KYC with the help of an Aadhar card.  At the time of enrolment, farmers have to provide all the regarding land. Land details are available on the revenue department website.</t>
+  </si>
+  <si>
+    <t>बिरसा किसान योजना झारखंड 2023, पंजीकरण, फॉर्म (Birsa Kisan Yojana Jharkhand)</t>
+  </si>
+  <si>
+    <t>7. Meethi Kranti Yojana (Sweet Revolution Scheme)</t>
+  </si>
+  <si>
+    <t>A scheme for farmers called as Meethi Kranti Yojana (Sweet Revolution Scheme). Bee keeping training along with the unit worth Rs. 1 lakh will be given by the government. Farmers can start a side business of bee keeping &amp; selling honey. Rs. 80,000 will be given as a grant where as farmers needs to invest Rs. 20,000. The objective of the scheme is to qua</t>
+  </si>
+  <si>
+    <t>Sweet Revolution (Mithi Kranti)- Steps towards doubling farmers Income - MyGov Blogs</t>
+  </si>
+  <si>
+    <t>8. Interest Free Farm Loan Scheme</t>
+  </si>
+  <si>
+    <t>Jharkhand farmers will now get farm loan on zero percent interest rate. Jharkhand Government has made an announcement of the Interest Free Farm Loan Scheme. The interest free loan is only for the first year and hence farmers needs to pay the loan in 1st year. The interest for the loan for the first year will be paid by the government. If farmers cannot repay in one year then he needs to pay interest rate on the agricultural loan.</t>
+  </si>
+  <si>
+    <t>https://www.indiafilings.com/learn/interest-free-farm-loan-scheme/</t>
+  </si>
+  <si>
+    <t>9. Attracting &amp; Retaining Youth in Agriculture (ARYA) Scheme</t>
+  </si>
+  <si>
+    <t>To engage and encourage Youth in Agriculture, the Government of Jharkhand has launched Attracting and Retaining Youth in Agriculture (ARYA) Scheme for the youth. Under the ARYA scheme, the state government attract rural youth in agriculture by providing them skill training and make the state self-dependent in agriculture. The aim is to engaging youth in agriculture and promotes the green revolution in the state. In this scheme, Agriculture Technology Management and Training (ATMA) provide training to the rural youth in the state and for this, two youths from each village selected for the training. Selected youth will get training about agriculture like how to properly use of barren land, uncultivated land, and inspired youth to grow food grains. Agriculture is one of the pre-eminent sectors of Jharkhand’s rural economy. The Agriculture and Allied sector has recorded an impressive average annual growth of above 5 percent between 2011-12 and 2015-16. Such type of scheme helps and encourage youth towards agriculture sector and Jharkhand government took excellent initiatives for the future</t>
+  </si>
+  <si>
+    <t>https://ataribengaluru.icar.gov.in/docs/pub/2.pdf</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh</t>
+  </si>
+  <si>
+    <t>Prakritik Kheti Khushaal Kisan Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote organic farming and provide financial assistance to farmers to adopt organic farming practices. The scheme covers the cost of organic inputs and provides a subsidy for organic farming equipment.</t>
+  </si>
+  <si>
+    <t>The applicant must be a farmer or a group of farmers practicing agriculture in Himachal Pradesh. The landholding of the farmer should not exceed 5 acres.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/prakritik-kheti-khushhal-kisan-yojna/</t>
+  </si>
+  <si>
+    <t>Mukhya Mantri Khet Sanrakshan Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to farmers for the construction of protective structures such as barbed wire fencing, stone walls, and trenches to protect their crops from wild animals.</t>
+  </si>
+  <si>
+    <t>The applicant must be a farmer practicing agriculture in Himachal Pradesh.</t>
+  </si>
+  <si>
+    <t>https://hpgeneralstudies.com/what-is-mukhya-mantri-khet-sanrakshan-yojana/</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh Horticulture Development Project</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote the horticulture sector in Himachal Pradesh by providing financial assistance for the establishment of orchards, the adoption of modern farming techniques, and the creation of post-harvest infrastructure.</t>
+  </si>
+  <si>
+    <t>The applicant must be a farmer or a group of farmers practicing horticulture in Himachal Pradesh. The landholding of the farmer should not exceed 5 acres.</t>
+  </si>
+  <si>
+    <t>https://hds.hp.gov.in/GeneralpageWithTemplate.aspx?key=HOMEKEY0001</t>
+  </si>
+  <si>
+    <t>Mukhya Mantri Greenhouse
+Renovation Scheme (MMGRS)</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote greenhouse farming in Himachal Pradesh by providing financial assistance for the construction of greenhouses and purchase of equipment for climate control.</t>
+  </si>
+  <si>
+    <t>The applicant must be a farmer practicing agriculture in Himachal Pradesh. The landholding of the farmer should not exceed 1 acre.</t>
+  </si>
+  <si>
+    <t>https://eudyan.hp.gov.in/UploadedImages/Document/Mukhya%20Mantri%20Green%20House%20Renovation%20Scheme.pdf</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh Agriculture Marketing Board</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide a market for agricultural produce and ensure fair prices to farmers in Himachal Pradesh. The scheme covers the construction of market yards, grading and sorting facilities, and transportation facilities for agricultural produce.</t>
+  </si>
+  <si>
+    <t>The applicant must be a farmer or a group of farmers practicing agriculture in Himachal Pradesh.</t>
+  </si>
+  <si>
+    <t>https://www.hpsamb.org/</t>
+  </si>
+  <si>
+    <t>Flow Irrigation Scheme</t>
+  </si>
+  <si>
+    <t>The Follow Irrigation Scheme aims to promote efficient water management in agriculture by providing financial assistance for the establishment of follow irrigation systems. Follow irrigation is a technique where irrigation water is applied to one crop, and the excess water is used to irrigate the next crop downstream. This technique helps in conserving water and improving the efficiency of water use. The scheme covers the cost of follow irrigation systems, including pipelines, pumps, and other necessary equipment.</t>
+  </si>
+  <si>
+    <t>The applicant must be a farmer practicing agriculture in Himachal Pradesh. The landholding of the farmer should not exceed 5 acres. The applicant must have a source of irrigation water and must be willing to adopt follow irrigation techniques. The scheme is applicable for all types of crops, including fruits, vegetables, and cereals.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/flow-irrigation-scheme/</t>
+  </si>
+  <si>
+    <t>Rajya Krishi Yantrikaran Programme</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance for the purchase of farm machinery and equipment to farmers in Himachal Pradesh. The scheme covers a subsidy for the purchase of tractors, power tillers, harvesters, and other agricultural equipment.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/state-agricultural-mechanisation/</t>
+  </si>
+  <si>
+    <t>Prakritik Kheti Khushhal Kisan Yojna</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote organic farming practices in Himachal Pradesh by providing financial assistance for the adoption of organic farming techniques, including composting, vermicomposting, and organic inputs. The scheme covers the cost of organic inputs, training and capacity building for farmers, and support for marketing and value addition activities.</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Kisaan evam Khetihar Mazdoor Jeevan Suraksha Yojna</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide life insurance cover to farmers and agricultural workers in Himachal Pradesh. The scheme covers accidental and natural death and provides financial assistance to the nominee in case of the death of the insured.</t>
+  </si>
+  <si>
+    <t>The applicant must be a farmer or agricultural worker practicing in Himachal Pradesh.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/mukhyamantri-kisaan-evam-khetihar-mazdoor-jeevan-suraksha-yojna/</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Nutan Polyhouse Pariyojna</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote protected cultivation practices in Himachal Pradesh by providing financial assistance for the establishment of polyhouses. The scheme covers the cost of the construction of polyhouses and other necessary equipment.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/mukhyamantri-nutan-polyhouse-pariyojna/</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Krishi Utpadan Sanrakshan Yojna</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to farmers for the purchase of crop insurance to protect them from crop losses due to natural calamities and other unforeseen events. The scheme covers crop losses due to floods, droughts, landslides, and other natural calamities.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/mukhya-mantri-krishi-utpadan-sanrakshan-yojna/</t>
+  </si>
+  <si>
+    <t>Krishi se Sampannta Yojna</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote the establishment of agriculture-related industries in Himachal Pradesh by providing financial assistance for the establishment of agro-processing units, storage facilities, and marketing infrastructure.</t>
+  </si>
+  <si>
+    <t>The applicant must be an entrepreneur or a group of entrepreneurs planning to establish an agriculture-related industry in Himachal Pradesh.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/krishi-se-sampannta-yojna/</t>
+  </si>
+  <si>
+    <t>Jal se Krishi ko Bal Yojna</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote efficient water management in agriculture by providing financial assistance for the establishment of micro-irrigation systems, including drip irrigation and sprinkler irrigation. The scheme covers the cost of micro-irrigation systems, including pipelines, pumps, and other necessary equipment.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/jal-se-krishi-ko-bal-yojna/</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Krishi Samvardhan Yojna</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote the development of agriculture and horticulture sectors in Himachal Pradesh by providing financial assistance for the establishment of irrigation facilities, water conservation measures, and land development activities.</t>
+  </si>
+  <si>
+    <t>The applicant must be a farmer practicing agriculture or horticulture in Himachal Pradesh.</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/mukhya-mantri-krishi-samvardhan-yojna/</t>
+  </si>
+  <si>
+    <t>Tea and Coffee Cultivation Scheme</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote the cultivation of tea and coffee in the Kangra valley of Himachal Pradesh by providing financial assistance for the establishment of tea and coffee plantations, processing units, and marketing infrastructure.</t>
+  </si>
+  <si>
+    <t>The applicant must be an entrepreneur or a group of entrepreneurs planning to establish a tea or coffee plantation in the</t>
+  </si>
+  <si>
+    <t>https://agriculture.hp.gov.in/en/our-scheme/tea-cultivation-scheme-cofee-production/</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>National Food Security Mission NFSM 60:40</t>
+  </si>
+  <si>
+    <t>To increase food grain production by providing technical and financial assistance to farmers in selected districts of Haryana</t>
+  </si>
+  <si>
+    <t>Farmers in selected districts of Haryana</t>
+  </si>
+  <si>
+    <t>https://www.nfsm.gov.in/</t>
+  </si>
+  <si>
+    <t>Rashtriya Krishi Vikas Yojana RKVY-RAFTAAR</t>
+  </si>
+  <si>
+    <t>To incentivize states to increase their agriculture and allied sector investment and improve overall performance in these sectors</t>
+  </si>
+  <si>
+    <t>Farmers and agricultural institutions in Haryana</t>
+  </si>
+  <si>
+    <t>https://www.manage.gov.in/managecia/RKVYProg.aspx</t>
+  </si>
+  <si>
+    <t>Reclamation of Saline soils and Waterlogged Land in the State</t>
+  </si>
+  <si>
+    <t>To reclaim and utilize saline and waterlogged land in Haryana for agricultural purposes</t>
+  </si>
+  <si>
+    <t>Farmers in Haryana with saline or waterlogged land</t>
+  </si>
+  <si>
+    <t>https://agriharyana.gov.in/hopp</t>
+  </si>
+  <si>
+    <t>Promotion of Summer Moong under CDP</t>
+  </si>
+  <si>
+    <t>To promote the cultivation of summer moong in Haryana through various interventions such as seed distribution, training, and technical assistance</t>
+  </si>
+  <si>
+    <t>Farmers in Haryana</t>
+  </si>
+  <si>
+    <t>https://agriharyana.gov.in/SummerMoong</t>
+  </si>
+  <si>
+    <t>Natural Farming - Promotion of Sustainable agriculture strategies initiative &amp; Kisan kalyan</t>
+  </si>
+  <si>
+    <t>To promote sustainable agriculture practices and provide financial assistance to farmers in Haryana</t>
+  </si>
+  <si>
+    <t>https://agriharyana.gov.in/naturalfarming</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Kisan Sahayata Yojana</t>
+  </si>
+  <si>
+    <t>To provide financial assistance to small and marginal farmers in Bihar</t>
+  </si>
+  <si>
+    <t>Small and marginal farmers in Bihar</t>
+  </si>
+  <si>
+    <t>https://pacsonline.bih.nic.in/fsy/login.aspx</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Harit Krishi Sanyantra Yojana</t>
+  </si>
+  <si>
+    <t>To provide subsidy for purchasing agriculture machinery to farmers in Bihar</t>
+  </si>
+  <si>
+    <t>Farmers in Bihar</t>
+  </si>
+  <si>
+    <t>https://www.indiafilings.com/learn/mukhyamantri-harit-krishi-sanyantra-yojana/</t>
+  </si>
+  <si>
+    <t>Bihar Kisan Credit Card Scheme</t>
+  </si>
+  <si>
+    <t>To provide credit facilities to farmers for agricultural and allied activities in Bihar</t>
+  </si>
+  <si>
+    <t>https://biharonlineportal.com/kisan-credit-card-online-apply/</t>
+  </si>
+  <si>
+    <t>Bihar Rajya Beej Nigam Limited</t>
+  </si>
+  <si>
+    <t>To ensure the availability of quality seeds to farmers in Bihar</t>
+  </si>
+  <si>
+    <t>https://brbn.bihar.gov.in/</t>
+  </si>
+  <si>
+    <t>Bihar Kisan Samman Nidhi Yojana</t>
+  </si>
+  <si>
+    <t>To provide financial assistance to farmers in Bihar for the purchase of inputs and for agricultural operations</t>
+  </si>
+  <si>
+    <t>https://dbtagriculture.bihar.gov.in/PMKisan/Print_PMKISANNew.aspx</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Nischay Schemes</t>
+  </si>
+  <si>
+    <t>Various schemes under Mukhyamantri Nischay Yojana to provide assistance to farmers for agriculture and allied activities in Bihar</t>
+  </si>
+  <si>
+    <t>https://www.7nishchay-yuvaupmission.bihar.gov.in/</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Rythu Bharosa Scheme</t>
+  </si>
+  <si>
+    <t>The applicant must be a resident of Andhra Pradesh.
+The applicant must be a small and marginal farmer with less than 5 acres of agricultural land.
+The applicant must have a valid identification document such as an Aadhaar card or Voter ID.</t>
+  </si>
+  <si>
+    <t>Rythu Bharosa is a financial assistance scheme for farmers launched by the Government of Andhra Pradesh. Eligible farmers will receive financial assistance of Rs. 13,500 per year. The eligibility criteria include</t>
+  </si>
+  <si>
+    <t>https://ysrrythubharosa.ap.gov.in/RBApp/index.html</t>
+  </si>
+  <si>
+    <t>Zero-Budget Natural Farming (ZBNF)</t>
+  </si>
+  <si>
+    <t>Zero-Budget Natural Farming is a farming method where farmers use natural resources such as cow dung, urine, and other organic matter as fertilizers and pest control agents. The Government of Andhra Pradesh has launched a scheme to promote ZBNF among farmers.</t>
+  </si>
+  <si>
+    <t>The farmer must be a resident of Andhra Pradesh.
+The farmer must own land and be actively involved in farming.
+The farmer must have a willingness to adopt ZBNF practices.</t>
+  </si>
+  <si>
+    <t>https://zbnf.org.in/</t>
+  </si>
+  <si>
+    <t>YSR Pension Scheme</t>
+  </si>
+  <si>
+    <t>The YSR Pension Scheme is a financial assistance scheme for old age people, widows, and disabled people in Andhra Pradesh. Farmers who fall under these categories are eligible for this scheme</t>
+  </si>
+  <si>
+    <t>The farmer must be a resident of Andhra Pradesh.
+The farmer must be over 60 years old (for old age pension), widowed, or disabled.
+The farmer must have a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://sspensions.ap.gov.in/SSP</t>
+  </si>
+  <si>
+    <t>PM Kisan Samman Nidhi Yojana</t>
+  </si>
+  <si>
+    <t>PM Kisan Samman Nidhi Yojana is a central government scheme launched to provide financial assistance to small and marginal farmers in India.</t>
+  </si>
+  <si>
+    <t>The farmer must be a resident of India.
+The farmer must own land and be actively involved in farming.
+The farmer's landholding must be less than 2 hectares.
+The farmer must have a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>National Mission on Oilseeds and Oil Palm (NMOOP)</t>
+  </si>
+  <si>
+    <t>National Mission on Oilseeds and Oil Palm is a scheme launched by the Government of India to increase the production of oilseeds and oil palm in the country.</t>
+  </si>
+  <si>
+    <t>The farmer must be a resident of India.
+The farmer must own land and be actively involved in farming.
+The farmer must be interested in cultivating oilseeds or oil palm.</t>
+  </si>
+  <si>
+    <t>https://nmeo.dac.gov.in/</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Kisan Kalyan Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to farmers in the state of Madhya Pradesh for various purposes such as crop insurance, soil health improvement, seeds and fertilizers, and irrigation facilities.</t>
+  </si>
+  <si>
+    <t>Eligibility criteria include being a resident of Madhya Pradesh, owning or cultivating agricultural land, and possessing a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://mpkrishi.mp.gov.in/hindisite_New/indexEnglish_New.aspx</t>
+  </si>
+  <si>
+    <t>Krishi Rin Samadhan Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide relief to farmers in the state of Madhya Pradesh who are burdened with debt by providing them with loan waivers and a one-time settlement scheme.</t>
+  </si>
+  <si>
+    <t>Eligibility criteria include being a resident of Madhya Pradesh, owning agricultural land, having a maximum outstanding loan of up to Rs. 2 lakh as of March 31, 2018, and possessing a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://apexbank.in/</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Krishak Jeevan Kalyan Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to the family members of farmers who die or become permanently disabled while performing agricultural activities.</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to farmers in the state of Madhya Pradesh for crop loss due to natural calamities such as floods, droughts, and unseasonal rains.</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Yuva Swabhiman Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to unemployed youth in the state of Madhya Pradesh for starting their own agriculture-related businesses.</t>
+  </si>
+  <si>
+    <t>Eligibility criteria include being a resident of Madhya Pradesh, being between the ages of 18 and 45, having completed at least 10th standard education, and possessing a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>Chattisgarh</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Krishak Sarvhit Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to farmers in the state of Chhattisgarh for various purposes such as crop insurance, soil health improvement, seeds and fertilizers, and irrigation facilities.</t>
+  </si>
+  <si>
+    <t>The applicant must be a resident of Chhattisgarh.
+The applicant must own or cultivate agricultural land.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://agriportal.cg.nic.in/PortHi/</t>
+  </si>
+  <si>
+    <t>Pradhan Mantri Fasal Bima Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide insurance coverage and financial assistance to farmers in case of crop failure due to natural calamities such as floods, droughts, and pest attacks.</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Baagbaan Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote horticulture in the state of Chhattisgarh by providing financial assistance for setting up horticulture farms and nurseries.</t>
+  </si>
+  <si>
+    <t>Applicant must be a resident of Chhattisgarh.
+Applicant must own or lease agricultural land for at least 5 years.
+Applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://agriportal.cg.nic.in/horticulture/HortiEn/Default.aspx</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Mahila Kisan Swarozgar Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to empower women farmers in the state of Chhattisgarh by providing financial assistance for setting up their own agriculture-related businesses.</t>
+  </si>
+  <si>
+    <t>Chhattisgarh State Agriculture Development Scheme</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote agricultural development in the state of Chhattisgarh by providing financial assistance for various purposes such as crop cultivation, irrigation facilities, and farm mechanization.</t>
+  </si>
+  <si>
+    <t>Applicant must be a resident of Chhattisgarh.
+Applicant must be a woman farmer.
+Applicant must have completed at least 10th standard education.
+Applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>Applicant must be a resident of Chhattisgarh.
+Applicant must own or cultivate agricultural land.
+Applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>Rythu Bandhu Scheme</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to farmers to support their investment in agriculture and allied activities.</t>
+  </si>
+  <si>
+    <t>Applicant must be a farmer who owns cultivable land in Telangana.
+The land must be registered under the name of the applicant.
+The land must be used for agricultural activities.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>http://rythubandhu.telangana.gov.in/</t>
+  </si>
+  <si>
+    <t>Mission Bhagiratha</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide safe drinking water to rural households in Telangana.</t>
+  </si>
+  <si>
+    <t>Applicant must be a resident of rural Telangana.
+The applicant's household must be located in a village where the scheme is being implemented.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://missionbhagiratha.telangana.gov.in/</t>
+  </si>
+  <si>
+    <t>Sheep Distribution Scheme</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to sheep and goat farmers in Telangana for the purchase of animals.</t>
+  </si>
+  <si>
+    <t>Applicant must be a farmer who owns sheep or goat.
+The applicant must have experience in sheep or goat farming.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://cm.telangana.gov.in/2019/06/sheep-distribution/</t>
+  </si>
+  <si>
+    <t>Telangana State Agriculture Development</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to farmers for the development of agriculture and allied activities.</t>
+  </si>
+  <si>
+    <t>Applicant must be a farmer who owns or cultivates agricultural land in Telangana.
+The land must be registered under the name of the applicant.
+The land must be used for agricultural activities.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://agri.telangana.gov.in/</t>
+  </si>
+  <si>
+    <t>Mission Kakatiya</t>
+  </si>
+  <si>
+    <t>This scheme aims to restore and rejuvenate the water tanks and irrigation systems in Telangana.</t>
+  </si>
+  <si>
+    <t>Applicant must be a resident of rural Telangana.
+The applicant's land must be irrigated by the tanks and irrigation systems under the scheme.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://missionkakatiya.cgg.gov.in/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,19 +1119,154 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Google Sans"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F7F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD9D9E3"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD9D9E3"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -511,7 +1276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -524,6 +1289,135 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -540,6 +1434,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -839,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EB68AB-D548-4777-AFB4-3B1C26B4199A}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:AA86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="83" zoomScaleNormal="47" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,7 +1769,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -888,7 +1786,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -922,7 +1820,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -939,7 +1837,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -956,7 +1854,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -973,7 +1871,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +1973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1094,7 +1992,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1113,7 +2011,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="288" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1130,7 +2028,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -1149,7 +2047,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -1168,7 +2066,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1187,7 +2085,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1391,7 +2289,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -1406,6 +2304,1446 @@
       </c>
       <c r="E32" s="4" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="9"/>
+      <c r="Y33" s="9"/>
+      <c r="Z33" s="9"/>
+      <c r="AA33" s="9"/>
+    </row>
+    <row r="34" spans="1:27" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="12"/>
+      <c r="Y34" s="12"/>
+      <c r="Z34" s="12"/>
+      <c r="AA34" s="12"/>
+    </row>
+    <row r="35" spans="1:27" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="16"/>
+      <c r="Z35" s="16"/>
+      <c r="AA35" s="16"/>
+    </row>
+    <row r="36" spans="1:27" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="20"/>
+    </row>
+    <row r="37" spans="1:27" ht="106.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
+      <c r="U37" s="24"/>
+      <c r="V37" s="24"/>
+      <c r="W37" s="24"/>
+      <c r="X37" s="24"/>
+      <c r="Y37" s="24"/>
+      <c r="Z37" s="24"/>
+      <c r="AA37" s="24"/>
+    </row>
+    <row r="38" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="28"/>
+      <c r="E38" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="28"/>
+      <c r="S38" s="28"/>
+      <c r="T38" s="28"/>
+      <c r="U38" s="28"/>
+      <c r="V38" s="28"/>
+      <c r="W38" s="28"/>
+      <c r="X38" s="28"/>
+      <c r="Y38" s="28"/>
+      <c r="Z38" s="28"/>
+      <c r="AA38" s="28"/>
+    </row>
+    <row r="39" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="28"/>
+      <c r="E39" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="28"/>
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
+      <c r="Z39" s="28"/>
+      <c r="AA39" s="28"/>
+    </row>
+    <row r="40" spans="1:27" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" s="28"/>
+      <c r="E40" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="28"/>
+      <c r="W40" s="28"/>
+      <c r="X40" s="28"/>
+      <c r="Y40" s="28"/>
+      <c r="Z40" s="28"/>
+      <c r="AA40" s="28"/>
+    </row>
+    <row r="41" spans="1:27" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27"/>
+      <c r="U41" s="27"/>
+      <c r="V41" s="27"/>
+      <c r="W41" s="27"/>
+      <c r="X41" s="27"/>
+      <c r="Y41" s="27"/>
+      <c r="Z41" s="27"/>
+      <c r="AA41" s="27"/>
+    </row>
+    <row r="42" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="E42" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
+      <c r="O42" s="34"/>
+      <c r="P42" s="34"/>
+      <c r="Q42" s="34"/>
+      <c r="R42" s="34"/>
+      <c r="S42" s="34"/>
+      <c r="T42" s="34"/>
+      <c r="U42" s="34"/>
+      <c r="V42" s="34"/>
+      <c r="W42" s="34"/>
+      <c r="X42" s="34"/>
+      <c r="Y42" s="34"/>
+      <c r="Z42" s="34"/>
+      <c r="AA42" s="34"/>
+    </row>
+    <row r="43" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="37"/>
+      <c r="N43" s="37"/>
+      <c r="O43" s="37"/>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37"/>
+      <c r="U43" s="37"/>
+      <c r="V43" s="37"/>
+      <c r="W43" s="37"/>
+      <c r="X43" s="37"/>
+      <c r="Y43" s="37"/>
+      <c r="Z43" s="37"/>
+      <c r="AA43" s="37"/>
+    </row>
+    <row r="44" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="40"/>
+      <c r="O44" s="40"/>
+      <c r="P44" s="40"/>
+      <c r="Q44" s="40"/>
+      <c r="R44" s="40"/>
+      <c r="S44" s="40"/>
+      <c r="T44" s="40"/>
+      <c r="U44" s="40"/>
+      <c r="V44" s="40"/>
+      <c r="W44" s="40"/>
+      <c r="X44" s="40"/>
+      <c r="Y44" s="40"/>
+      <c r="Z44" s="40"/>
+      <c r="AA44" s="40"/>
+    </row>
+    <row r="45" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D45" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="43"/>
+      <c r="O45" s="43"/>
+      <c r="P45" s="43"/>
+      <c r="Q45" s="43"/>
+      <c r="R45" s="43"/>
+      <c r="S45" s="43"/>
+      <c r="T45" s="43"/>
+      <c r="U45" s="43"/>
+      <c r="V45" s="43"/>
+      <c r="W45" s="43"/>
+      <c r="X45" s="43"/>
+      <c r="Y45" s="43"/>
+      <c r="Z45" s="43"/>
+      <c r="AA45" s="43"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A46" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="E46" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="43"/>
+      <c r="O46" s="43"/>
+      <c r="P46" s="43"/>
+      <c r="Q46" s="43"/>
+      <c r="R46" s="43"/>
+      <c r="S46" s="43"/>
+      <c r="T46" s="43"/>
+      <c r="U46" s="43"/>
+      <c r="V46" s="43"/>
+      <c r="W46" s="43"/>
+      <c r="X46" s="43"/>
+      <c r="Y46" s="43"/>
+      <c r="Z46" s="43"/>
+      <c r="AA46" s="43"/>
+    </row>
+    <row r="47" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+      <c r="N47" s="43"/>
+      <c r="O47" s="43"/>
+      <c r="P47" s="43"/>
+      <c r="Q47" s="43"/>
+      <c r="R47" s="43"/>
+      <c r="S47" s="43"/>
+      <c r="T47" s="43"/>
+      <c r="U47" s="43"/>
+      <c r="V47" s="43"/>
+      <c r="W47" s="43"/>
+      <c r="X47" s="43"/>
+      <c r="Y47" s="43"/>
+      <c r="Z47" s="43"/>
+      <c r="AA47" s="43"/>
+    </row>
+    <row r="48" spans="1:27" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
+      <c r="N48" s="43"/>
+      <c r="O48" s="43"/>
+      <c r="P48" s="43"/>
+      <c r="Q48" s="43"/>
+      <c r="R48" s="43"/>
+      <c r="S48" s="43"/>
+      <c r="T48" s="43"/>
+      <c r="U48" s="43"/>
+      <c r="V48" s="43"/>
+      <c r="W48" s="43"/>
+      <c r="X48" s="43"/>
+      <c r="Y48" s="43"/>
+      <c r="Z48" s="43"/>
+      <c r="AA48" s="43"/>
+    </row>
+    <row r="49" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="43"/>
+      <c r="O49" s="43"/>
+      <c r="P49" s="43"/>
+      <c r="Q49" s="43"/>
+      <c r="R49" s="43"/>
+      <c r="S49" s="43"/>
+      <c r="T49" s="43"/>
+      <c r="U49" s="43"/>
+      <c r="V49" s="43"/>
+      <c r="W49" s="43"/>
+      <c r="X49" s="43"/>
+      <c r="Y49" s="43"/>
+      <c r="Z49" s="43"/>
+      <c r="AA49" s="43"/>
+    </row>
+    <row r="50" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="D50" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E50" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="43"/>
+      <c r="M50" s="43"/>
+      <c r="N50" s="43"/>
+      <c r="O50" s="43"/>
+      <c r="P50" s="43"/>
+      <c r="Q50" s="43"/>
+      <c r="R50" s="43"/>
+      <c r="S50" s="43"/>
+      <c r="T50" s="43"/>
+      <c r="U50" s="43"/>
+      <c r="V50" s="43"/>
+      <c r="W50" s="43"/>
+      <c r="X50" s="43"/>
+      <c r="Y50" s="43"/>
+      <c r="Z50" s="43"/>
+      <c r="AA50" s="43"/>
+    </row>
+    <row r="51" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="D51" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="43"/>
+      <c r="M51" s="43"/>
+      <c r="N51" s="43"/>
+      <c r="O51" s="43"/>
+      <c r="P51" s="43"/>
+      <c r="Q51" s="43"/>
+      <c r="R51" s="43"/>
+      <c r="S51" s="43"/>
+      <c r="T51" s="43"/>
+      <c r="U51" s="43"/>
+      <c r="V51" s="43"/>
+      <c r="W51" s="43"/>
+      <c r="X51" s="43"/>
+      <c r="Y51" s="43"/>
+      <c r="Z51" s="43"/>
+      <c r="AA51" s="43"/>
+    </row>
+    <row r="52" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="D52" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="E52" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="49"/>
+      <c r="J52" s="49"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="49"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="49"/>
+      <c r="O52" s="49"/>
+      <c r="P52" s="49"/>
+      <c r="Q52" s="49"/>
+      <c r="R52" s="49"/>
+      <c r="S52" s="49"/>
+      <c r="T52" s="49"/>
+      <c r="U52" s="49"/>
+      <c r="V52" s="49"/>
+      <c r="W52" s="49"/>
+      <c r="X52" s="49"/>
+      <c r="Y52" s="49"/>
+      <c r="Z52" s="49"/>
+      <c r="AA52" s="49"/>
+    </row>
+    <row r="53" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="C53" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="D53" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="49"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="49"/>
+      <c r="O53" s="49"/>
+      <c r="P53" s="49"/>
+      <c r="Q53" s="49"/>
+      <c r="R53" s="49"/>
+      <c r="S53" s="49"/>
+      <c r="T53" s="49"/>
+      <c r="U53" s="49"/>
+      <c r="V53" s="49"/>
+      <c r="W53" s="49"/>
+      <c r="X53" s="49"/>
+      <c r="Y53" s="49"/>
+      <c r="Z53" s="49"/>
+      <c r="AA53" s="49"/>
+    </row>
+    <row r="54" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C54" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="E54" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="49"/>
+      <c r="L54" s="49"/>
+      <c r="M54" s="49"/>
+      <c r="N54" s="49"/>
+      <c r="O54" s="49"/>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
+      <c r="R54" s="49"/>
+      <c r="S54" s="49"/>
+      <c r="T54" s="49"/>
+      <c r="U54" s="49"/>
+      <c r="V54" s="49"/>
+      <c r="W54" s="49"/>
+      <c r="X54" s="49"/>
+      <c r="Y54" s="49"/>
+      <c r="Z54" s="49"/>
+      <c r="AA54" s="49"/>
+    </row>
+    <row r="55" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="D55" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="E55" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="49"/>
+      <c r="N55" s="49"/>
+      <c r="O55" s="49"/>
+      <c r="P55" s="49"/>
+      <c r="Q55" s="49"/>
+      <c r="R55" s="49"/>
+      <c r="S55" s="49"/>
+      <c r="T55" s="49"/>
+      <c r="U55" s="49"/>
+      <c r="V55" s="49"/>
+      <c r="W55" s="49"/>
+      <c r="X55" s="49"/>
+      <c r="Y55" s="49"/>
+      <c r="Z55" s="49"/>
+      <c r="AA55" s="49"/>
+    </row>
+    <row r="56" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B56" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="E56" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+    </row>
+    <row r="57" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B57" s="52" t="s">
+        <v>199</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="D57" s="53" t="s">
+        <v>201</v>
+      </c>
+      <c r="E57" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49"/>
+    </row>
+    <row r="58" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="C58" s="52" t="s">
+        <v>204</v>
+      </c>
+      <c r="D58" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F58" s="55"/>
+      <c r="G58" s="56"/>
+    </row>
+    <row r="59" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B59" s="52" t="s">
+        <v>207</v>
+      </c>
+      <c r="C59" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="D59" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F59" s="54"/>
+      <c r="G59" s="57"/>
+    </row>
+    <row r="60" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B60" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="C60" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="D60" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F60" s="58"/>
+      <c r="G60" s="59"/>
+    </row>
+    <row r="61" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B61" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="C61" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="D61" s="53" t="s">
+        <v>217</v>
+      </c>
+      <c r="E61" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+    </row>
+    <row r="62" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B62" s="52" t="s">
+        <v>219</v>
+      </c>
+      <c r="C62" s="52" t="s">
+        <v>220</v>
+      </c>
+      <c r="D62" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="E62" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
+    </row>
+    <row r="63" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B63" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="C63" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="D63" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="E63" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+    </row>
+    <row r="64" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B64" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="C64" s="52" t="s">
+        <v>227</v>
+      </c>
+      <c r="D64" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="E64" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B65" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="C65" s="52" t="s">
+        <v>230</v>
+      </c>
+      <c r="D65" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="E65" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+    </row>
+    <row r="66" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B66" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" s="52" t="s">
+        <v>233</v>
+      </c>
+      <c r="D66" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="E66" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49"/>
+    </row>
+    <row r="67" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>235</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E67" s="51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E68" s="50" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E69" s="50" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E70" s="51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E71" s="51" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>255</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E72" s="51" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="49" t="s">
+        <v>255</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E73" s="51" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A74" s="49" t="s">
+        <v>255</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E74" s="51" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="49" t="s">
+        <v>255</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E75" s="51" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="49" t="s">
+        <v>255</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E76" s="51" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>270</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E77" s="51" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="49" t="s">
+        <v>270</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E78" s="51" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A79" s="49" t="s">
+        <v>270</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E79" s="51" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="49" t="s">
+        <v>270</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E80" s="51" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A81" s="49" t="s">
+        <v>270</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E81" s="51" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>287</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E82" s="51" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E83" s="51" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A84" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E84" s="51" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E85" s="51" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E86" s="51" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -1441,9 +3779,63 @@
     <hyperlink ref="E30" r:id="rId29" xr:uid="{EDF017E9-5491-48E4-BA18-5B4DAC15CA6E}"/>
     <hyperlink ref="E31" r:id="rId30" xr:uid="{0E0D11CB-F34A-4675-BE68-9D32B6A2FF91}"/>
     <hyperlink ref="E32" r:id="rId31" xr:uid="{5C626202-B02A-458E-BC2E-CC2042515F3C}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{01174F56-F2AF-484B-9F59-F3AF3DE0A6B9}"/>
+    <hyperlink ref="E34" r:id="rId33" location=":~:text=31%20%E0%A4%AE%E0%A4%BE%E0%A4%B0%E0%A5%8D%E0%A4%9A%2C%202020%20%E0%A4%A4%E0%A4%95%20%E0%A4%95%E0%A5%87,%E0%A4%95%E0%A4%AE%20%E0%A4%B8%E0%A5%87%20%E0%A4%95%E0%A4%AE%20%E0%A4%B8%E0%A4%AE%E0%A5%8D%E0%A4%AA%E0%A4%B0%E0%A5%8D%E0%A4%95%20%E0%A4%B9%E0%A5%8B%E0%A4%97%E0%A4%BE%E0%A5%A4" display="https://jkrmy.jharkhand.gov.in/ - :~:text=31%20%E0%A4%AE%E0%A4%BE%E0%A4%B0%E0%A5%8D%E0%A4%9A%2C%202020%20%E0%A4%A4%E0%A4%95%20%E0%A4%95%E0%A5%87,%E0%A4%95%E0%A4%AE%20%E0%A4%B8%E0%A5%87%20%E0%A4%95%E0%A4%AE%20%E0%A4%B8%E0%A4%AE%E0%A5%8D%E0%A4%AA%E0%A4%B0%E0%A5%8D%E0%A4%95%20%E0%A4%B9%E0%A5%8B%E0%A4%97%E0%A4%BE%E0%A5%A4" xr:uid="{D1B1C042-D8D1-473A-ABDC-B3937743BC25}"/>
+    <hyperlink ref="E35" r:id="rId34" location=":~:text=%E0%A4%9D%E0%A4%BE%E0%A4%B0%E0%A4%96%E0%A4%A3%E0%A5%8D%E0%A4%A1%20%E0%A4%B0%E0%A4%BE%E0%A4%9C%E0%A5%8D%E0%A4%AF%20%E0%A4%AB%E0%A4%B8%E0%A4%B2%20%E0%A4%B0%E0%A4%BE%E0%A4%B9%E0%A4%A4%20%E0%A4%AF%E0%A5%8B%E0%A4%9C%E0%A4%A8%E0%A4%BE%20(JRFRY)%20%E0%A4%AB%E0%A4%B8%E0%A4%B2%20%E0%A4%AC%E0%A5%80%E0%A4%AE%E0%A4%BE%20%E0%A4%AF%E0%A5%8B%E0%A4%9C%E0%A4%A8%E0%A4%BE%20%E0%A4%A8,%E0%A4%95%E0%A5%87%20%E0%A4%B8%E0%A4%82%E0%A4%95%E0%A4%B2%E0%A5%8D%E0%A4%AA%20%E0%A4%95%E0%A5%8B%20%E0%A4%AA%E0%A5%82%E0%A4%B0%E0%A4%BE%20%E0%A4%95%E0%A4%B0%E0%A5%87%E0%A4%97%E0%A4%BE%E0%A5%A4" display="https://jrfry.jharkhand.gov.in/ - :~:text=%E0%A4%9D%E0%A4%BE%E0%A4%B0%E0%A4%96%E0%A4%A3%E0%A5%8D%E0%A4%A1%20%E0%A4%B0%E0%A4%BE%E0%A4%9C%E0%A5%8D%E0%A4%AF%20%E0%A4%AB%E0%A4%B8%E0%A4%B2%20%E0%A4%B0%E0%A4%BE%E0%A4%B9%E0%A4%A4%20%E0%A4%AF%E0%A5%8B%E0%A4%9C%E0%A4%A8%E0%A4%BE%20(JRFRY)%20%E0%A4%AB%E0%A4%B8%E0%A4%B2%20%E0%A4%AC%E0%A5%80%E0%A4%AE%E0%A4%BE%20%E0%A4%AF%E0%A5%8B%E0%A4%9C%E0%A4%A8%E0%A4%BE%20%E0%A4%A8,%E0%A4%95%E0%A5%87%20%E0%A4%B8%E0%A4%82%E0%A4%95%E0%A4%B2%E0%A5%8D%E0%A4%AA%20%E0%A4%95%E0%A5%8B%20%E0%A4%AA%E0%A5%82%E0%A4%B0%E0%A4%BE%20%E0%A4%95%E0%A4%B0%E0%A5%87%E0%A4%97%E0%A4%BE%E0%A5%A4" xr:uid="{9D35282C-475B-424B-9E0C-A12715DE03D6}"/>
+    <hyperlink ref="E36" r:id="rId35" location=":~:text=%E0%A4%B8%E0%A4%AE%E0%A5%87%E0%A4%95%E0%A4%BF%E0%A4%A4%20%E0%A4%AC%E0%A4%BF%E0%A4%B0%E0%A4%B8%E0%A4%BE%20%E0%A4%97%E0%A5%8D%E0%A4%B0%E0%A4%BE%E0%A4%AE%20%E0%A4%B5%E0%A4%BF%E0%A4%95%E0%A4%BE%E0%A4%B8%20%E0%A4%AF%E0%A5%8B%E0%A4%9C%E0%A4%A8%E0%A4%BE%20%E0%A4%95%E0%A5%87%20%E0%A4%A4%E0%A4%B9%E0%A4%A4%20%E0%A4%AA%E0%A5%8D%E0%A4%B0%E0%A4%A4%E0%A5%8D%E0%A4%AF%E0%A5%87%E0%A4%95%20%E0%A4%9C%E0%A4%BF%E0%A4%B2%E0%A5%87%20%E0%A4%B8%E0%A5%87,%E0%A4%95%E0%A5%80%20%E0%A4%86%E0%A4%AF%20%E0%A4%AE%E0%A5%87%E0%A4%82%20%E0%A4%AC%E0%A4%A2%E0%A4%BC%E0%A5%8B%E0%A4%A4%E0%A5%8D%E0%A4%A4%E0%A4%B0%E0%A5%80%20%E0%A4%B9%E0%A5%8B%E0%A4%97%E0%A5%80%E0%A5%A4" display="https://sarkariyojana.com/samekit-birsa-gram-vikas-yojana/ - :~:text=%E0%A4%B8%E0%A4%AE%E0%A5%87%E0%A4%95%E0%A4%BF%E0%A4%A4%20%E0%A4%AC%E0%A4%BF%E0%A4%B0%E0%A4%B8%E0%A4%BE%20%E0%A4%97%E0%A5%8D%E0%A4%B0%E0%A4%BE%E0%A4%AE%20%E0%A4%B5%E0%A4%BF%E0%A4%95%E0%A4%BE%E0%A4%B8%20%E0%A4%AF%E0%A5%8B%E0%A4%9C%E0%A4%A8%E0%A4%BE%20%E0%A4%95%E0%A5%87%20%E0%A4%A4%E0%A4%B9%E0%A4%A4%20%E0%A4%AA%E0%A5%8D%E0%A4%B0%E0%A4%A4%E0%A5%8D%E0%A4%AF%E0%A5%87%E0%A4%95%20%E0%A4%9C%E0%A4%BF%E0%A4%B2%E0%A5%87%20%E0%A4%B8%E0%A5%87,%E0%A4%95%E0%A5%80%20%E0%A4%86%E0%A4%AF%20%E0%A4%AE%E0%A5%87%E0%A4%82%20%E0%A4%AC%E0%A4%A2%E0%A4%BC%E0%A5%8B%E0%A4%A4%E0%A5%8D%E0%A4%A4%E0%A4%B0%E0%A5%80%20%E0%A4%B9%E0%A5%8B%E0%A4%97%E0%A5%80%E0%A5%A4" xr:uid="{F1374E48-FD44-4243-9029-A479BB7C0CC2}"/>
+    <hyperlink ref="E37" r:id="rId36" location=":~:text=Birsa%20Kisan%20Yojana%20Jharkhand%20Benefit&amp;text=%E0%A4%87%E0%A4%B8%20%E0%A4%AF%E0%A5%8B%E0%A4%9C%E0%A4%A8%E0%A4%BE%20%E0%A4%95%E0%A5%87%20%E0%A4%86%E0%A4%A8%E0%A5%87%20%E0%A4%B8%E0%A5%87,%E0%A4%95%E0%A4%BE%E0%A4%AE%E0%A5%8B%E0%A4%82%20%E0%A4%AE%E0%A5%87%E0%A4%82%20%E0%A4%95%E0%A4%B0%20%E0%A4%B8%E0%A4%95%E0%A4%A4%E0%A5%87%20%E0%A4%B9%E0%A5%88%E0%A4%82." display="https://www.yojanaschemehindi.com/birsa-kisan-jharkhand-registration-form/ - :~:text=Birsa%20Kisan%20Yojana%20Jharkhand%20Benefit&amp;text=%E0%A4%87%E0%A4%B8%20%E0%A4%AF%E0%A5%8B%E0%A4%9C%E0%A4%A8%E0%A4%BE%20%E0%A4%95%E0%A5%87%20%E0%A4%86%E0%A4%A8%E0%A5%87%20%E0%A4%B8%E0%A5%87,%E0%A4%95%E0%A4%BE%E0%A4%AE%E0%A5%8B%E0%A4%82%20%E0%A4%AE%E0%A5%87%E0%A4%82%20%E0%A4%95%E0%A4%B0%20%E0%A4%B8%E0%A4%95%E0%A4%A4%E0%A5%87%20%E0%A4%B9%E0%A5%88%E0%A4%82." xr:uid="{FACF6F78-9ED7-4C47-A055-24FC882F96BA}"/>
+    <hyperlink ref="E38" r:id="rId37" display="https://blog.mygov.in/sweet-revolution-mithi-kranti-steps-towards-doubling-farmers-income/" xr:uid="{366E8461-C0BF-4E4B-A75E-F63DF02867A2}"/>
+    <hyperlink ref="E39" r:id="rId38" xr:uid="{F07A5AF4-77AD-44DF-ACFD-6958D7D26378}"/>
+    <hyperlink ref="E40" r:id="rId39" xr:uid="{6E252F95-F968-4D28-9CA9-9A39A27B9DEE}"/>
+    <hyperlink ref="E51" r:id="rId40" xr:uid="{67EBFAF7-8CE6-4AFD-916C-9E621465CDFB}"/>
+    <hyperlink ref="E47" r:id="rId41" xr:uid="{55F5ED7B-621A-47F3-A1F3-F924112F2475}"/>
+    <hyperlink ref="E48" r:id="rId42" xr:uid="{CA3BC82D-BF21-4088-9F00-00AE6127253B}"/>
+    <hyperlink ref="E53" r:id="rId43" xr:uid="{523DAA2E-2DA4-4AC2-BC37-8326E718DFE6}"/>
+    <hyperlink ref="E52" r:id="rId44" xr:uid="{D5C4BC2F-A3F7-4776-B197-1A6B7CFA9C3E}"/>
+    <hyperlink ref="E54" r:id="rId45" xr:uid="{C04F3463-3E06-459D-ACB6-A2FFE239914F}"/>
+    <hyperlink ref="E55" r:id="rId46" xr:uid="{180DEB18-496A-441F-AC8B-5AED69C1CD2C}"/>
+    <hyperlink ref="E56" r:id="rId47" xr:uid="{5CADD3AB-2CA9-48AB-9855-29607C687BC0}"/>
+    <hyperlink ref="E57" r:id="rId48" xr:uid="{3CBD284C-1C08-4371-9CA7-122087E8A203}"/>
+    <hyperlink ref="E58" r:id="rId49" xr:uid="{32CDC8FB-6616-4527-93ED-933BCE4112B7}"/>
+    <hyperlink ref="E59" r:id="rId50" xr:uid="{F29D8453-3076-4746-BD55-0B7FD45A8CE7}"/>
+    <hyperlink ref="E60" r:id="rId51" xr:uid="{059377D1-6D00-4B89-869F-D45368283BBF}"/>
+    <hyperlink ref="E61" r:id="rId52" xr:uid="{DA15FACF-EB43-45A9-859E-8D88FD4A513A}"/>
+    <hyperlink ref="E62" r:id="rId53" xr:uid="{E7E4782A-1763-4476-A2DB-13901B1BEB15}"/>
+    <hyperlink ref="E64" r:id="rId54" xr:uid="{F4ACBA3F-E786-4100-A25D-2558BF876886}"/>
+    <hyperlink ref="E65" r:id="rId55" xr:uid="{1B962C5B-6667-46A0-8405-B1D61536D906}"/>
+    <hyperlink ref="E63" r:id="rId56" xr:uid="{F43801C0-932A-4974-ACB6-270DB412CF24}"/>
+    <hyperlink ref="E66" r:id="rId57" xr:uid="{308CA0F2-3AD3-4EBA-995D-E2580E4462F6}"/>
+    <hyperlink ref="E67" r:id="rId58" xr:uid="{EC5D9301-DACF-4837-BDC5-27122B9023AB}"/>
+    <hyperlink ref="E68" r:id="rId59" xr:uid="{97E25978-F66D-4846-B88C-DE7D08652DB7}"/>
+    <hyperlink ref="E69" r:id="rId60" xr:uid="{C97A730E-BA6C-473F-ADF3-1B0B88CAA26B}"/>
+    <hyperlink ref="E70" r:id="rId61" xr:uid="{00BD0B7D-72CA-4BF4-8775-96ED92C0E58E}"/>
+    <hyperlink ref="E71" r:id="rId62" xr:uid="{5F632E63-A08A-4066-A63B-216774C3E364}"/>
+    <hyperlink ref="E72" r:id="rId63" xr:uid="{3985669C-A76E-4034-B3D8-74D71C3D965B}"/>
+    <hyperlink ref="E73" r:id="rId64" xr:uid="{35ECD6EF-2630-43B6-83D9-ABFD8DECA80B}"/>
+    <hyperlink ref="E74" r:id="rId65" xr:uid="{811C5943-BF3C-4819-B647-E31BE0498BFC}"/>
+    <hyperlink ref="E75" r:id="rId66" xr:uid="{EF015AC0-B4FA-41C6-AF0B-5F20F5E7918F}"/>
+    <hyperlink ref="E76" r:id="rId67" xr:uid="{C78F459A-2DBF-46FC-8007-803DB7ED0C10}"/>
+    <hyperlink ref="E77" r:id="rId68" xr:uid="{3D9D6384-907A-4A3F-8851-8E9C2945AB2D}"/>
+    <hyperlink ref="E78" r:id="rId69" xr:uid="{B06C7D75-9F43-41EB-8A81-101E013961E3}"/>
+    <hyperlink ref="E79" r:id="rId70" xr:uid="{F5C85470-FDC0-417C-8625-2B1EBDE89BC0}"/>
+    <hyperlink ref="E80" r:id="rId71" xr:uid="{7259F410-CD92-442F-99F7-B02FADA65356}"/>
+    <hyperlink ref="E81" r:id="rId72" xr:uid="{D4EA4883-3A08-48C7-ABA3-D3F596684B8D}"/>
+    <hyperlink ref="E82" r:id="rId73" xr:uid="{AE90DE3A-4B2D-4228-95D6-11C08CC3EBE3}"/>
+    <hyperlink ref="E83" r:id="rId74" xr:uid="{BC9D2D80-61E0-4102-B41A-D9189F4153DE}"/>
+    <hyperlink ref="E84" r:id="rId75" xr:uid="{D29447B9-135E-4C81-AA59-090D6FC5F600}"/>
+    <hyperlink ref="E85" r:id="rId76" xr:uid="{431DCAC2-C301-4CBF-B9BC-22F7F1BD1AE8}"/>
+    <hyperlink ref="E86" r:id="rId77" xr:uid="{6A9CD428-AAF1-4037-B825-CC827329E8F5}"/>
+    <hyperlink ref="E41" r:id="rId78" xr:uid="{BAAF8A4E-7D3C-44C6-B45C-3AFB1C4E247A}"/>
+    <hyperlink ref="E42" r:id="rId79" xr:uid="{A743A92F-6E8E-4AE4-9627-7AEB5DBDD6CA}"/>
+    <hyperlink ref="E43" r:id="rId80" xr:uid="{E4229FD3-65BA-4295-8519-709F055719A1}"/>
+    <hyperlink ref="E44" r:id="rId81" xr:uid="{D813D1B3-E9DB-48DA-AF0B-4E0E93A65DCA}"/>
+    <hyperlink ref="E45" r:id="rId82" xr:uid="{9709C078-E75F-4AB8-B596-A32A7FEF8FAC}"/>
+    <hyperlink ref="E46" r:id="rId83" xr:uid="{CB9AFBD2-2016-47F4-A101-FC61F822B036}"/>
+    <hyperlink ref="E49" r:id="rId84" xr:uid="{FA3D8241-3756-4DA1-87E7-C74699704A80}"/>
+    <hyperlink ref="E50" r:id="rId85" xr:uid="{DD7B1248-6D8C-4877-B4D4-904219781023}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId86"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">

</xml_diff>

<commit_message>
Added 8 more states
</commit_message>
<xml_diff>
--- a/govt aided schemes/govt_schemes.xlsx
+++ b/govt aided schemes/govt_schemes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41c4ab87885fd82d/Desktop/AgroInOne/govt aided schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="14_{33830C7A-9471-4095-8464-0F557495317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F797D837-1117-4FCB-BB16-0799E7264E96}"/>
+  <xr:revisionPtr revIDLastSave="389" documentId="14_{33830C7A-9471-4095-8464-0F557495317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D1656FF-1F92-4997-AC3B-D9CB598AAECF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD2C649B-7986-471F-8B6F-2885A4982D96}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="523">
   <si>
     <t>All India</t>
   </si>
@@ -1092,12 +1092,684 @@
   <si>
     <t>https://missionkakatiya.cgg.gov.in/</t>
   </si>
+  <si>
+    <t>Meghalaya</t>
+  </si>
+  <si>
+    <t>All farmers who have taken a crop loan from any bank are eligible to apply for this scheme. The scheme provides insurance cover for crops in case of natural calamities, pests, or diseases.</t>
+  </si>
+  <si>
+    <t>Meghalaya State Crop Insurance Scheme</t>
+  </si>
+  <si>
+    <t>All farmers in the state who have insurable interest in the crop are eligible to apply for this scheme. The scheme provides insurance cover for crops in case of natural calamities, pests, or diseases.</t>
+  </si>
+  <si>
+    <t>https://meghalaya.gov.in/schemes?page=3</t>
+  </si>
+  <si>
+    <t>Meghalaya Horticulture Mission</t>
+  </si>
+  <si>
+    <t>https://mbda.gov.in/horticulture-mission</t>
+  </si>
+  <si>
+    <t>Farmers, groups of farmers, and self-help groups involved in horticulture activities are eligible to apply for this scheme. The scheme provides financial assistance for setting up horticulture farms, purchase of machinery, and for capacity building.</t>
+  </si>
+  <si>
+    <t>Meghalaya Milk Mission</t>
+  </si>
+  <si>
+    <t>https://megahvt.gov.in/megh_milk_mission.html</t>
+  </si>
+  <si>
+    <t>Dairy farmers, self-help groups, and milk cooperatives are eligible to apply for this scheme. The scheme provides financial assistance for setting up milk processing plants, purchase of machinery, and for capacity building.</t>
+  </si>
+  <si>
+    <t>Meghalaya State Agricultural Mechanization Programme</t>
+  </si>
+  <si>
+    <t>https://megagriculture.gov.in/FarmMech/SECURE/FM_Login.aspx</t>
+  </si>
+  <si>
+    <t>Farmers, groups of farmers, and self-help groups are eligible to apply for this scheme. The scheme provides financial assistance for purchase of farm machinery, such as tractors, tillers, and harvesters.</t>
+  </si>
+  <si>
+    <t>This scheme is a crop insurance scheme introduced by the Government of India to provide insurance cover for crops in case of natural calamities, pests, or diseases.</t>
+  </si>
+  <si>
+    <t>This is a state-level crop insurance scheme that provides insurance cover for crops in case of natural calamities, pests, or diseases.</t>
+  </si>
+  <si>
+    <t>This scheme is aimed at promoting horticulture in Meghalaya by providing financial assistance to farmers, groups of farmers, and self-help groups involved in horticulture activities. The assistance is provided for setting up horticulture farms, purchase of machinery, and for capacity building.</t>
+  </si>
+  <si>
+    <t>This scheme is aimed at promoting dairy farming in Meghalaya by providing financial assistance to dairy farmers, self-help groups, and milk cooperatives. The assistance is provided for setting up milk processing plants, purchase of machinery, and for capacity building.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This scheme is aimed at promoting the use of farm machinery in Meghalaya by providing financial assistance to farmers, groups of farmers, and self-help groups. The assistance is provided for purchase of farm machinery, such as tractors, tillers, and harvesters. </t>
+  </si>
+  <si>
+    <t>Tripura</t>
+  </si>
+  <si>
+    <t>Mukhyamantri Fasal Bima Yojana</t>
+  </si>
+  <si>
+    <t>To provide insurance coverage to farmers in Tripura for losses due to natural calamities</t>
+  </si>
+  <si>
+    <t>Farmers in Tripura</t>
+  </si>
+  <si>
+    <t>https://www.tripuraindia.in/index.php?/update/index/mukhya-mantri-fasal-bima-yojna--announced-in-tripura-to-protect-4-42-lakh-farmers</t>
+  </si>
+  <si>
+    <t>Chief Minister's Irrigation Assistance Scheme</t>
+  </si>
+  <si>
+    <t>To provide subsidy for the installation of micro-irrigation systems to farmers in Tripura</t>
+  </si>
+  <si>
+    <t>https://pwd.tripura.gov.in/index.php/other-wings/pwd-wr</t>
+  </si>
+  <si>
+    <t>Chief Minister's Livestock Development Scheme</t>
+  </si>
+  <si>
+    <t>To provide financial assistance to farmers for the development of livestock in Tripura</t>
+  </si>
+  <si>
+    <t>https://ardd.tripura.gov.in/?q=tlda</t>
+  </si>
+  <si>
+    <t>Chief Minister's Agricultural Entrepreneurship Scheme</t>
+  </si>
+  <si>
+    <t>To provide financial assistance to agri-entrepreneurs in Tripura for setting up agri-businesses</t>
+  </si>
+  <si>
+    <t>Agri-entrepreneurs in Tripura</t>
+  </si>
+  <si>
+    <t>https://affairscloud.com/tripura-government-launches-agro-entrepreneur-facilitation-desk-to-boost-economy/</t>
+  </si>
+  <si>
+    <t>Chief Minister's Floriculture Development Scheme</t>
+  </si>
+  <si>
+    <t>To promote the development of floriculture in Tripura by providing financial assistance to farmers</t>
+  </si>
+  <si>
+    <t>https://horti.tripura.gov.in/sites/default/files/mukhyamantri-puspa-udhyan-prakalpya.pdf</t>
+  </si>
+  <si>
+    <t>Tripura State Co-operative Bank Kisan Credit Card Scheme</t>
+  </si>
+  <si>
+    <t>To provide credit facilities to farmers for agricultural and allied activities in Tripura</t>
+  </si>
+  <si>
+    <t>https://tscbank.nic.in/kcc.htm</t>
+  </si>
+  <si>
+    <t>Chief Minister's Organic Mission Scheme</t>
+  </si>
+  <si>
+    <t>To promote organic farming practices and provide financial assistance to farmers in Tripura</t>
+  </si>
+  <si>
+    <t>https://agricoop.nic.in/sites/default/files/movcdner_revised.pdf</t>
+  </si>
+  <si>
+    <t>Tripura Green Mission</t>
+  </si>
+  <si>
+    <t>To promote the development of agroforestry, horticulture, and plantation crops in Tripura by providing financial assistance to farmers</t>
+  </si>
+  <si>
+    <t>https://forest.tripura.gov.in/forest-scheme?id=MQ==</t>
+  </si>
+  <si>
+    <t>Tripura State Horticulture Mission</t>
+  </si>
+  <si>
+    <t>To promote horticulture and floriculture in Tripura by providing technical and financial assistance to farmers</t>
+  </si>
+  <si>
+    <t>https://horti.tripura.gov.in/tshm</t>
+  </si>
+  <si>
+    <t>Mizoram</t>
+  </si>
+  <si>
+    <t>Rashtriya Krishi Vikas Yojana</t>
+  </si>
+  <si>
+    <t>To promote the development of agriculture and allied sectors in Mizoram by providing financial assistance for various activities such as crop development, horticulture, and livestock development</t>
+  </si>
+  <si>
+    <t>Farmers and agri-entrepreneurs in Mizoram</t>
+  </si>
+  <si>
+    <t>https://agriculturemizoram.nic.in/pages/rkvy.html</t>
+  </si>
+  <si>
+    <t>State Agricultural Management &amp; Extension Training Institute (SAMETI)</t>
+  </si>
+  <si>
+    <t>To provide training and capacity building to farmers, extension workers, and other stakeholders in Mizoram for the development of agriculture and allied sectors</t>
+  </si>
+  <si>
+    <t>Farmers, extension workers, and other stakeholders in Mizoram</t>
+  </si>
+  <si>
+    <t>https://agriculturemizoram.nic.in/pages/sameti.html</t>
+  </si>
+  <si>
+    <t>OIL PALM CULTIVATION IN MIZORAM</t>
+  </si>
+  <si>
+    <t>To promote the cultivation of oil palm in Mizoram and provide financial assistance to farmers for the same</t>
+  </si>
+  <si>
+    <t>Farmers in Mizoram</t>
+  </si>
+  <si>
+    <t>https://agriculturemizoram.nic.in/pages/oilpalm.html</t>
+  </si>
+  <si>
+    <t>KRISHI VIGYAN KENDRA MIZORAM</t>
+  </si>
+  <si>
+    <t>To provide technical assistance and training to farmers in Mizoram for the development of agriculture and allied sectors</t>
+  </si>
+  <si>
+    <t>https://agriculturemizoram.nic.in/pages/kvk.html</t>
+  </si>
+  <si>
+    <t>PLANT PROTECTION</t>
+  </si>
+  <si>
+    <t>To promote plant protection measures and provide technical assistance to farmers in Mizoram for pest and disease management</t>
+  </si>
+  <si>
+    <t>https://agriculturemizoram.nic.in/pages/plantprotection.html</t>
+  </si>
+  <si>
+    <t>Fostering Climate Resilient Upland Farming System</t>
+  </si>
+  <si>
+    <t>To promote climate-resilient farming practices and provide financial assistance to farmers in Mizoram for the same</t>
+  </si>
+  <si>
+    <t>https://agriculturemizoram.nic.in/pages/focus.html</t>
+  </si>
+  <si>
+    <t>Green-Ag</t>
+  </si>
+  <si>
+    <t>To promote sustainable agriculture practices and provide financial assistance to farmers in Mizoram for the adoption of such practices</t>
+  </si>
+  <si>
+    <t>https://agriculturemizoram.nic.in/pages/greenag.html</t>
+  </si>
+  <si>
+    <t>Sub-Mission on Agroforestry (SMAF)</t>
+  </si>
+  <si>
+    <t>To promote agroforestry in Mizoram and provide financial assistance to farmers for setting up agroforestry systems</t>
+  </si>
+  <si>
+    <t>https://agriculturemizoram.nic.in/pages/smaf.html</t>
+  </si>
+  <si>
+    <t>Nagaland</t>
+  </si>
+  <si>
+    <t>NORTH EAST REGION AGRI EXPO</t>
+  </si>
+  <si>
+    <t>To promote agriculture and allied sectors in Nagaland by providing a platform for showcasing and selling agricultural products</t>
+  </si>
+  <si>
+    <t>Farmers and agri-entrepreneurs in Nagaland</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/north-east-agri-expo/</t>
+  </si>
+  <si>
+    <t>RAINFED AREA DEVELOPMENT (RAD) UNDER NMSA</t>
+  </si>
+  <si>
+    <t>To promote sustainable rainfed farming practices in Nagaland and provide financial assistance to farmers for the same</t>
+  </si>
+  <si>
+    <t>Farmers in Nagaland</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/rainfed-area-developmentrad-under-nmsa/</t>
+  </si>
+  <si>
+    <t>SEED PRODUCTION PROGRAMME (RKVY)</t>
+  </si>
+  <si>
+    <t>To promote seed production and provide financial assistance to farmers for setting up seed production units in Nagaland</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/seed-production-programme-rkvy/</t>
+  </si>
+  <si>
+    <t>FARM MECHANIZATION UNDER SMAM &amp; RKVY</t>
+  </si>
+  <si>
+    <t>To promote farm mechanization in Nagaland and provide financial assistance to farmers for the purchase of agricultural machinery and equipment</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/smam/</t>
+  </si>
+  <si>
+    <t>WOMEN IN AGRICULTURE</t>
+  </si>
+  <si>
+    <t>To promote the participation of women in agriculture and provide training and financial assistance to women farmers in Nagaland</t>
+  </si>
+  <si>
+    <t>Women farmers in Nagaland</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/women-in-agriculture/</t>
+  </si>
+  <si>
+    <t>STRENGTHENING AND MODERNIZATION OF PEST MANAGEMENT APPROACH IN INDIA (SMPP)</t>
+  </si>
+  <si>
+    <t>To promote modern and sustainable pest management practices in Nagaland and provide technical assistance to farmers for the same</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/strengthening-and-modernization-of-pest-management/</t>
+  </si>
+  <si>
+    <t>AGRICULTURE CENSUS SCHEME</t>
+  </si>
+  <si>
+    <t>To conduct agriculture census in Nagaland and collect data on various aspects of agriculture and allied sectors</t>
+  </si>
+  <si>
+    <t>Farmers and agricultural workers in Nagaland</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/activities-of-the-department/agriculture-census/</t>
+  </si>
+  <si>
+    <t>Agriculture Technology Management Agency (ATMA)</t>
+  </si>
+  <si>
+    <t>To provide technical assistance and training to farmers in Nagaland for the development of agriculture and allied sectors</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/atma/</t>
+  </si>
+  <si>
+    <t>INTEGRATED NUTRIENT MANAGEMENT</t>
+  </si>
+  <si>
+    <t>To promote integrated nutrient management practices in Nagaland and provide financial assistance to farmers for the same</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/integrated-nutrient-management/</t>
+  </si>
+  <si>
+    <t>BRIEF DESCRIPTION OF THE PROJECT (RIDF-XIX)</t>
+  </si>
+  <si>
+    <t>To provide financial assistance for various agriculture and allied sector projects in Nagaland</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/brief-description-of-the-project-ridf-xix/</t>
+  </si>
+  <si>
+    <t>EDUCATION &amp; TRAINING</t>
+  </si>
+  <si>
+    <t>To provide education and training to farmers and other stakeholders in Nagaland for the development of agriculture and allied sectors</t>
+  </si>
+  <si>
+    <t>Farmers and other stakeholders in Nagaland</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/education-and-training/</t>
+  </si>
+  <si>
+    <t>AGRICULTURAL ECONOMICS AND STATISTICS</t>
+  </si>
+  <si>
+    <t>To conduct research and collect data on various aspects of agriculture and allied sectors in Nagaland</t>
+  </si>
+  <si>
+    <t>Researchers and agricultural workers in Nagaland</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/eras/</t>
+  </si>
+  <si>
+    <t>INTEGRATED PEST MANAGEMENT (RKVY)</t>
+  </si>
+  <si>
+    <t>To promote integrated pest management practices in Nagaland and provide financial assistance to farmers for the same</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/integrated-pest-managementrkvy/</t>
+  </si>
+  <si>
+    <t>JHUM-FALLOW MANAGEMENT</t>
+  </si>
+  <si>
+    <t>To promote sustainable jhum-fallow management practices in Nagaland and provide financial assistance to farmers for the same</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/jhum-fallow-management/</t>
+  </si>
+  <si>
+    <t>MISSION ORGANIC VALUE CHAIN DEVELOPMENT FOR NORTH EASTERN REGION (MoVCD)</t>
+  </si>
+  <si>
+    <t>To promote organic farming practices and provide financial assistance to farmers in Nagaland for the same</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/movcd/</t>
+  </si>
+  <si>
+    <t>NATIONAL FOOD SECURITY MISSION (NFSM)</t>
+  </si>
+  <si>
+    <t>To promote food security and increase agricultural productivity in Nagaland by providing financial assistance for various activities such as crop development, horticulture, and livestock development</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/nfsm/</t>
+  </si>
+  <si>
+    <t>NATIONAL MISSION ON OILSEEDS AND OIL PALM (NMOOP)</t>
+  </si>
+  <si>
+    <t>To promote the cultivation of oilseeds and oil palm in Nagaland and provide financial assistance to farmers for the same</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/nmoop/</t>
+  </si>
+  <si>
+    <t>“PRADHAN MANTRI KRISHI SINCHAYEE YOJANA” (PMKSY) and “PER DROP MORE CROP” OTHER INTERVENTIONS</t>
+  </si>
+  <si>
+    <t>To promote efficient water use in agriculture in Nagaland and provide financial</t>
+  </si>
+  <si>
+    <t>https://agriculture.nagaland.gov.in/pmksy/</t>
+  </si>
+  <si>
+    <t>Sikkim</t>
+  </si>
+  <si>
+    <t>National Food Security Mission</t>
+  </si>
+  <si>
+    <t>The National Food Security Mission (NFSM) is a centrally-sponsored scheme aimed at increasing the production of rice, wheat, and pulses in the country. The scheme provides financial assistance to farmers for the adoption of improved technologies and practices to increase crop productivity.</t>
+  </si>
+  <si>
+    <t>Farmers, landless laborers, and agricultural workers.</t>
+  </si>
+  <si>
+    <t>https://www.sikkimagrisnet.org/General/Eng/Schemes.aspx?ID=14</t>
+  </si>
+  <si>
+    <t>Extension Reforms</t>
+  </si>
+  <si>
+    <t>The Extension Reforms scheme is aimed at improving the agricultural extension system in the country. The scheme provides financial assistance to extension workers for training and capacity building. It also supports the establishment of Farmer Resource Centers (FRCs) to provide farmers with access to information on modern agricultural practices.</t>
+  </si>
+  <si>
+    <t>Farmers and extension workers.</t>
+  </si>
+  <si>
+    <t>Agriculture Census</t>
+  </si>
+  <si>
+    <t>The Agriculture Census is a nationwide survey aimed at collecting data on agricultural practices in the country. The survey is conducted every five years and provides information on various aspects of agriculture such as land use, cropping patterns, irrigation facilities, and livestock.</t>
+  </si>
+  <si>
+    <t>Farmers and agricultural workers.</t>
+  </si>
+  <si>
+    <t>Scheme Test2</t>
+  </si>
+  <si>
+    <t>No information available.</t>
+  </si>
+  <si>
+    <t>test Schem1</t>
+  </si>
+  <si>
+    <t>Construction of godown and Office Building of Melli Dara MPCS</t>
+  </si>
+  <si>
+    <t>The scheme aims to provide storage facilities for agricultural produce to reduce post-harvest losses. The scheme provides financial assistance to agricultural cooperatives for the construction of godowns and office buildings.</t>
+  </si>
+  <si>
+    <t>Farmers and agricultural cooperatives.</t>
+  </si>
+  <si>
+    <t>EARAS (Establishment of Agency for Reporting Agriculture Stat</t>
+  </si>
+  <si>
+    <t>The scheme aims to establish a system for collecting and reporting agricultural data at the village level. The scheme provides financial assistance for the establishment of an agency for reporting agricultural statistics (EARAS) at the district level.</t>
+  </si>
+  <si>
+    <t>HCM Package for Dry and Backward areas</t>
+  </si>
+  <si>
+    <t>The HCM (Horticulture, Cultivation, and Marketing) Package is aimed at providing financial assistance to farmers in dry and backward areas for the cultivation of horticulture crops. The scheme provides support for the establishment of nurseries, drip irrigation systems, and other modern agricultural practices.</t>
+  </si>
+  <si>
+    <t>Farmers in dry and backward areas.</t>
+  </si>
+  <si>
+    <t>Integrated Pest Management</t>
+  </si>
+  <si>
+    <t>The Integrated Pest Management (IPM) scheme aims to promote the use of integrated pest management practices in agriculture. The scheme provides financial assistance for the adoption of IPM practices such as biological control, use of pheromone traps, and crop rotation.</t>
+  </si>
+  <si>
+    <t>Initiative for Nutritional Security through Intensive Promoti</t>
+  </si>
+  <si>
+    <t>The scheme aims to improve food and nutritional security by promoting intensive agriculture practices. The scheme provides financial assistance to farmers for the adoption of modern agricultural practices such as high-yielding varieties, drip irrigation, and integrated pest management.</t>
+  </si>
+  <si>
+    <t>Farmers and landless laborers.</t>
+  </si>
+  <si>
+    <t>Soil Health Management</t>
+  </si>
+  <si>
+    <t>The Soil Health Management (SHM) scheme aims to improve soil health and fertility. The scheme provides financial assistance for the adoption of practices such as soil testing, use of organic fertilizers, and crop rotation.</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>Mukhya Mantri Krishi Sa-Sajuli Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to farmers for the purchase of farm machinery and equipment.</t>
+  </si>
+  <si>
+    <t>Applicant must be a farmer who owns cultivable land in Assam.
+The land must be registered under the name of the applicant.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://diragri.assam.gov.in/schemes/mukhya-mantri-krishi-sa-sajuli-yozana</t>
+  </si>
+  <si>
+    <t>Chief Minister's Samagra Gramya Unnayan Yojana</t>
+  </si>
+  <si>
+    <t>https://mmscmsguy.assam.gov.in/</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance for the overall development of rural areas, including agriculture and allied activities.</t>
+  </si>
+  <si>
+    <t>Applicant must be a resident of a rural area in Assam.
+The applicant must belong to a Scheduled Caste or Scheduled Tribe.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide insurance coverage and financial support to farmers in case of crop failure due to natural calamities.</t>
+  </si>
+  <si>
+    <t>Applicant must be a farmer who owns cultivable land in Assam.
+The land must be registered under the name of the applicant.
+The applicant must have a crop loan account or a Kisan Credit Card.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>Chief Minister's Sashakt Kisan Yojana</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance to small and marginal farmers in Assam.</t>
+  </si>
+  <si>
+    <t>Applicant must be a small or marginal farmer who owns cultivable land in Assam.
+The land must be registered under the name of the applicant.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://westsiang.nic.in/scheme-category/chief-ministers-sashakt-kisan-yojana-cm-sky/</t>
+  </si>
+  <si>
+    <t>Assam Agribusiness and Rural Transformation Project</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide financial assistance and technical support for the development of agriculture and allied activities.</t>
+  </si>
+  <si>
+    <t>Applicant must be a farmer or agri-entrepreneur in Assam.
+The applicant must have a viable agribusiness plan.
+The applicant must possess a valid Aadhaar card.</t>
+  </si>
+  <si>
+    <t>https://dht.assam.gov.in/frontimpotentdata/assam-agribusiness-and-rural-transformation-project-apart</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>This scheme aims to provide insurance coverage and financial support to farmers in case of crop damage or loss due to natural calamities, pests, or diseases.</t>
+  </si>
+  <si>
+    <t>All farmers, including sharecroppers and tenant farmers, are eligible to enroll.
+The scheme covers all crops including horticulture crops, cereals, and oilseeds.
+The farmer should have a crop loan account or Kisan Credit Card.
+The scheme requires timely payment of premiums.</t>
+  </si>
+  <si>
+    <t>Farmers, farmer groups, cooperatives, and private sector organizations are eligible to apply.
+The scheme covers a range of activities including crop production, horticulture, animal husbandry, and fisheries.
+The proposed activities should be viable and have the potential to increase production and productivity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This scheme aims to promote agricultural development and increase agricultural productivity and income for farmers.</t>
+  </si>
+  <si>
+    <t>http://rkvy.nic.in/</t>
+  </si>
+  <si>
+    <t>This scheme aims to improve water use efficiency and increase the availability of water for agricultural purposes.</t>
+  </si>
+  <si>
+    <t>All farmers, including small and marginal farmers, are eligible to apply.
+The scheme covers activities such as creating and restoring water bodies, improving water distribution systems, and promoting water conservation.
+The proposed activities should be technically and economically viable.</t>
+  </si>
+  <si>
+    <t>http://pmksy.gov.in/</t>
+  </si>
+  <si>
+    <t>National Food Security Mission (NFSM)</t>
+  </si>
+  <si>
+    <t>This scheme aims to increase the production of rice, wheat, pulses, and coarse cereals and to ensure food security in the country.</t>
+  </si>
+  <si>
+    <t>Farmers, farmer groups, cooperatives, and private sector organizations are eligible to apply.
+The scheme covers activities such as seed distribution, soil testing, and the use of modern agricultural practices.
+The proposed activities should be aimed at increasing production and productivity.</t>
+  </si>
+  <si>
+    <t>This scheme aims to promote organic farming and to support farmers in adopting organic farming practices.</t>
+  </si>
+  <si>
+    <t>All farmers, including small and marginal farmers, are eligible to apply.
+The scheme covers activities such as the promotion of organic inputs, the use of traditional farming practices, and the creation of market linkages for organic produce.
+The proposed activities should be aimed at increasing production and productivity through organic farming practices.</t>
+  </si>
+  <si>
+    <t>https://dmsouthwest.delhi.gov.in/scheme/paramparagat-krishi-vikas-yojana/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arunachal </t>
+  </si>
+  <si>
+    <t>he Rashtriya Krishi Vikas Yojana aims to provide holistic development of agriculture and allied sectors by improving productivity, profitability, and sustainability of agriculture. This scheme is available to all farmers and aims to develop the agriculture sector through infrastructure development, seed development, and farm mechanization.</t>
+  </si>
+  <si>
+    <t>Farmers with landholding of up to 2 hectares can apply.
+Farmers should have a bank account.
+The scheme is available for both individual and group farmers.</t>
+  </si>
+  <si>
+    <t>https://agri.arunachal.gov.in/</t>
+  </si>
+  <si>
+    <t>Mission Organic Value Chain Development for North Eastern Region (MOVCD-NER)</t>
+  </si>
+  <si>
+    <t>Mission Organic Value Chain Development for North Eastern Region is a central government scheme that aims to promote organic farming in the North Eastern Region. The scheme provides support for the development of organic farming, certification, and market linkage for organic products.</t>
+  </si>
+  <si>
+    <t>All farmers in the North Eastern Region can apply for the scheme.
+The scheme is available for individual and group farmers.</t>
+  </si>
+  <si>
+    <t>https://agricoop.gov.in/#gsc.tab=0</t>
+  </si>
+  <si>
+    <t>The Pradhan Mantri Fasal Bima Yojana provides crop insurance coverage to farmers against crop loss due to natural calamities, pests, and diseases. The scheme aims to reduce the financial burden on farmers due to crop loss and provides them with the necessary support to continue farming.</t>
+  </si>
+  <si>
+    <t>All farmers who are cultivating notified crops in the state are eligible for the scheme.
+The scheme is available for both individual and group farmers.</t>
+  </si>
+  <si>
+    <t>The National Food Security Mission aims to increase the production of rice, wheat, and pulses in the country. The scheme provides support for seed distribution, farm mechanization, and soil health management.</t>
+  </si>
+  <si>
+    <t>All farmers in the state can apply for the scheme.
+The scheme is available for both individual and group farmers.</t>
+  </si>
+  <si>
+    <t>Sub-Mission on Agricultural Mechanization (SMAM)</t>
+  </si>
+  <si>
+    <t>The Sub-Mission on Agricultural Mechanization aims to promote the use of farm machinery to increase agricultural productivity and reduce the drudgery of farm operations. The scheme provides support for farm mechanization and the establishment of Custom Hiring Centers (CHCs).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1148,8 +1820,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF393939"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1174,8 +1852,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9EFED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1271,12 +1955,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1293,14 +1986,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1310,45 +1995,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1359,50 +2007,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1416,6 +2021,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1737,13 +2357,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EB68AB-D548-4777-AFB4-3B1C26B4199A}">
-  <dimension ref="A1:AA86"/>
+  <dimension ref="A1:AA152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="47" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="85" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.21875" customWidth="1"/>
     <col min="2" max="2" width="46.109375" style="2" customWidth="1"/>
@@ -1752,7 +2372,7 @@
     <col min="5" max="5" width="38.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1769,7 +2389,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="57.6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1786,7 +2406,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="72">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1803,7 +2423,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="72">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1820,7 +2440,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="72">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1837,7 +2457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="57.6">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +2474,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="86.4">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1871,7 +2491,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="86.4">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1888,7 +2508,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="144">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1905,7 +2525,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="172.8">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1922,7 +2542,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="288">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1939,7 +2559,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="288">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1956,7 +2576,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="288">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1973,7 +2593,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="57.6">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1992,7 +2612,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="72">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -2011,7 +2631,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="288">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -2028,7 +2648,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="57.6">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2047,7 +2667,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="72">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -2066,7 +2686,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="86.4">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2085,7 +2705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="216">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -2102,7 +2722,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="100.8">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -2119,7 +2739,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="100.8">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -2136,7 +2756,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="57.6">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -2153,7 +2773,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="57.6">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -2170,7 +2790,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="57.6">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2187,7 +2807,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="230.4">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -2204,7 +2824,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="159" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="159">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -2221,7 +2841,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="100.8">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -2238,7 +2858,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="72">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -2255,7 +2875,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="72">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -2272,7 +2892,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="100.8">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -2289,7 +2909,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="101.4" thickBot="1">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -2306,1107 +2926,762 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:27" ht="54" thickBot="1">
+      <c r="A33" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
-      <c r="AA33" s="9"/>
-    </row>
-    <row r="34" spans="1:27" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11" t="s">
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+      <c r="Z33" s="8"/>
+      <c r="AA33" s="8"/>
+    </row>
+    <row r="34" spans="1:27" ht="80.400000000000006" thickBot="1">
+      <c r="A34" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="12"/>
-      <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="12"/>
-      <c r="AA34" s="12"/>
-    </row>
-    <row r="35" spans="1:27" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="15" t="s">
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
+      <c r="AA34" s="8"/>
+    </row>
+    <row r="35" spans="1:27" ht="27.6" thickBot="1">
+      <c r="A35" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16"/>
-      <c r="W35" s="16"/>
-      <c r="X35" s="16"/>
-      <c r="Y35" s="16"/>
-      <c r="Z35" s="16"/>
-      <c r="AA35" s="16"/>
-    </row>
-    <row r="36" spans="1:27" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19" t="s">
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="8"/>
+      <c r="Z35" s="8"/>
+      <c r="AA35" s="8"/>
+    </row>
+    <row r="36" spans="1:27" ht="67.2" thickBot="1">
+      <c r="A36" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20"/>
-      <c r="S36" s="20"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="20"/>
-      <c r="X36" s="20"/>
-      <c r="Y36" s="20"/>
-      <c r="Z36" s="20"/>
-      <c r="AA36" s="20"/>
-    </row>
-    <row r="37" spans="1:27" ht="106.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="23" t="s">
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="8"/>
+      <c r="AA36" s="8"/>
+    </row>
+    <row r="37" spans="1:27" ht="106.8" thickBot="1">
+      <c r="A37" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="T37" s="24"/>
-      <c r="U37" s="24"/>
-      <c r="V37" s="24"/>
-      <c r="W37" s="24"/>
-      <c r="X37" s="24"/>
-      <c r="Y37" s="24"/>
-      <c r="Z37" s="24"/>
-      <c r="AA37" s="24"/>
-    </row>
-    <row r="38" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="27" t="s">
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="8"/>
+      <c r="AA37" s="8"/>
+    </row>
+    <row r="38" spans="1:27" ht="15" thickBot="1">
+      <c r="A38" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="29" t="s">
+      <c r="D38" s="8"/>
+      <c r="E38" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="28"/>
-      <c r="P38" s="28"/>
-      <c r="Q38" s="28"/>
-      <c r="R38" s="28"/>
-      <c r="S38" s="28"/>
-      <c r="T38" s="28"/>
-      <c r="U38" s="28"/>
-      <c r="V38" s="28"/>
-      <c r="W38" s="28"/>
-      <c r="X38" s="28"/>
-      <c r="Y38" s="28"/>
-      <c r="Z38" s="28"/>
-      <c r="AA38" s="28"/>
-    </row>
-    <row r="39" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="27" t="s">
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8"/>
+      <c r="AA38" s="8"/>
+    </row>
+    <row r="39" spans="1:27" ht="15" thickBot="1">
+      <c r="A39" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="31" t="s">
+      <c r="C39" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="29" t="s">
+      <c r="D39" s="8"/>
+      <c r="E39" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
-      <c r="O39" s="28"/>
-      <c r="P39" s="28"/>
-      <c r="Q39" s="28"/>
-      <c r="R39" s="28"/>
-      <c r="S39" s="28"/>
-      <c r="T39" s="28"/>
-      <c r="U39" s="28"/>
-      <c r="V39" s="28"/>
-      <c r="W39" s="28"/>
-      <c r="X39" s="28"/>
-      <c r="Y39" s="28"/>
-      <c r="Z39" s="28"/>
-      <c r="AA39" s="28"/>
-    </row>
-    <row r="40" spans="1:27" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="27" t="s">
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="8"/>
+    </row>
+    <row r="40" spans="1:27" ht="15" thickBot="1">
+      <c r="A40" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="29" t="s">
+      <c r="D40" s="8"/>
+      <c r="E40" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="28"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="Y40" s="28"/>
-      <c r="Z40" s="28"/>
-      <c r="AA40" s="28"/>
-    </row>
-    <row r="41" spans="1:27" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="27" t="s">
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="8"/>
+      <c r="AA40" s="8"/>
+    </row>
+    <row r="41" spans="1:27" ht="42" thickBot="1">
+      <c r="A41" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D41" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="E41" s="60" t="s">
+      <c r="E41" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="27"/>
-      <c r="Z41" s="27"/>
-      <c r="AA41" s="27"/>
-    </row>
-    <row r="42" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="34" t="s">
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:27" ht="28.2" thickBot="1">
+      <c r="A42" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D42" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="50" t="s">
+      <c r="E42" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="34"/>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
-      <c r="O42" s="34"/>
-      <c r="P42" s="34"/>
-      <c r="Q42" s="34"/>
-      <c r="R42" s="34"/>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
-      <c r="U42" s="34"/>
-      <c r="V42" s="34"/>
-      <c r="W42" s="34"/>
-      <c r="X42" s="34"/>
-      <c r="Y42" s="34"/>
-      <c r="Z42" s="34"/>
-      <c r="AA42" s="34"/>
-    </row>
-    <row r="43" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="37" t="s">
+    </row>
+    <row r="43" spans="1:27" ht="42" thickBot="1">
+      <c r="A43" t="s">
         <v>139</v>
       </c>
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="E43" s="50" t="s">
+      <c r="E43" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="37"/>
-      <c r="L43" s="37"/>
-      <c r="M43" s="37"/>
-      <c r="N43" s="37"/>
-      <c r="O43" s="37"/>
-      <c r="P43" s="37"/>
-      <c r="Q43" s="37"/>
-      <c r="R43" s="37"/>
-      <c r="S43" s="37"/>
-      <c r="T43" s="37"/>
-      <c r="U43" s="37"/>
-      <c r="V43" s="37"/>
-      <c r="W43" s="37"/>
-      <c r="X43" s="37"/>
-      <c r="Y43" s="37"/>
-      <c r="Z43" s="37"/>
-      <c r="AA43" s="37"/>
-    </row>
-    <row r="44" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="40" t="s">
+    </row>
+    <row r="44" spans="1:27" ht="28.2" thickBot="1">
+      <c r="A44" t="s">
         <v>139</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="E44" s="50" t="s">
+      <c r="E44" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="40"/>
-      <c r="N44" s="40"/>
-      <c r="O44" s="40"/>
-      <c r="P44" s="40"/>
-      <c r="Q44" s="40"/>
-      <c r="R44" s="40"/>
-      <c r="S44" s="40"/>
-      <c r="T44" s="40"/>
-      <c r="U44" s="40"/>
-      <c r="V44" s="40"/>
-      <c r="W44" s="40"/>
-      <c r="X44" s="40"/>
-      <c r="Y44" s="40"/>
-      <c r="Z44" s="40"/>
-      <c r="AA44" s="40"/>
-    </row>
-    <row r="45" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="43" t="s">
+    </row>
+    <row r="45" spans="1:27" ht="42" thickBot="1">
+      <c r="A45" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C45" s="46" t="s">
+      <c r="C45" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="47" t="s">
+      <c r="D45" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="E45" s="50" t="s">
+      <c r="E45" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="43"/>
-      <c r="O45" s="43"/>
-      <c r="P45" s="43"/>
-      <c r="Q45" s="43"/>
-      <c r="R45" s="43"/>
-      <c r="S45" s="43"/>
-      <c r="T45" s="43"/>
-      <c r="U45" s="43"/>
-      <c r="V45" s="43"/>
-      <c r="W45" s="43"/>
-      <c r="X45" s="43"/>
-      <c r="Y45" s="43"/>
-      <c r="Z45" s="43"/>
-      <c r="AA45" s="43"/>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+    </row>
+    <row r="46" spans="1:27">
+      <c r="A46" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C46" s="48" t="s">
+      <c r="C46" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="D46" s="48" t="s">
+      <c r="D46" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="E46" s="50" t="s">
+      <c r="E46" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="43"/>
-      <c r="P46" s="43"/>
-      <c r="Q46" s="43"/>
-      <c r="R46" s="43"/>
-      <c r="S46" s="43"/>
-      <c r="T46" s="43"/>
-      <c r="U46" s="43"/>
-      <c r="V46" s="43"/>
-      <c r="W46" s="43"/>
-      <c r="X46" s="43"/>
-      <c r="Y46" s="43"/>
-      <c r="Z46" s="43"/>
-      <c r="AA46" s="43"/>
-    </row>
-    <row r="47" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="43" t="s">
+    </row>
+    <row r="47" spans="1:27" ht="42" thickBot="1">
+      <c r="A47" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="46" t="s">
+      <c r="B47" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="C47" s="46" t="s">
+      <c r="C47" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="47" t="s">
+      <c r="D47" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E47" s="50" t="s">
+      <c r="E47" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="43"/>
-      <c r="O47" s="43"/>
-      <c r="P47" s="43"/>
-      <c r="Q47" s="43"/>
-      <c r="R47" s="43"/>
-      <c r="S47" s="43"/>
-      <c r="T47" s="43"/>
-      <c r="U47" s="43"/>
-      <c r="V47" s="43"/>
-      <c r="W47" s="43"/>
-      <c r="X47" s="43"/>
-      <c r="Y47" s="43"/>
-      <c r="Z47" s="43"/>
-      <c r="AA47" s="43"/>
-    </row>
-    <row r="48" spans="1:27" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="43" t="s">
+    </row>
+    <row r="48" spans="1:27" ht="55.8" thickBot="1">
+      <c r="A48" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="C48" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D48" s="47" t="s">
+      <c r="D48" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E48" s="45" t="s">
+      <c r="E48" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
-      <c r="M48" s="43"/>
-      <c r="N48" s="43"/>
-      <c r="O48" s="43"/>
-      <c r="P48" s="43"/>
-      <c r="Q48" s="43"/>
-      <c r="R48" s="43"/>
-      <c r="S48" s="43"/>
-      <c r="T48" s="43"/>
-      <c r="U48" s="43"/>
-      <c r="V48" s="43"/>
-      <c r="W48" s="43"/>
-      <c r="X48" s="43"/>
-      <c r="Y48" s="43"/>
-      <c r="Z48" s="43"/>
-      <c r="AA48" s="43"/>
-    </row>
-    <row r="49" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="43" t="s">
+    </row>
+    <row r="49" spans="1:7" ht="42" thickBot="1">
+      <c r="A49" t="s">
         <v>139</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="C49" s="46" t="s">
+      <c r="C49" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="D49" s="47" t="s">
+      <c r="D49" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="E49" s="50" t="s">
+      <c r="E49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="43"/>
-      <c r="O49" s="43"/>
-      <c r="P49" s="43"/>
-      <c r="Q49" s="43"/>
-      <c r="R49" s="43"/>
-      <c r="S49" s="43"/>
-      <c r="T49" s="43"/>
-      <c r="U49" s="43"/>
-      <c r="V49" s="43"/>
-      <c r="W49" s="43"/>
-      <c r="X49" s="43"/>
-      <c r="Y49" s="43"/>
-      <c r="Z49" s="43"/>
-      <c r="AA49" s="43"/>
-    </row>
-    <row r="50" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="43" t="s">
+    </row>
+    <row r="50" spans="1:7" ht="42" thickBot="1">
+      <c r="A50" t="s">
         <v>139</v>
       </c>
-      <c r="B50" s="46" t="s">
+      <c r="B50" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="C50" s="46" t="s">
+      <c r="C50" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D50" s="47" t="s">
+      <c r="D50" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="E50" s="50" t="s">
+      <c r="E50" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
-      <c r="M50" s="43"/>
-      <c r="N50" s="43"/>
-      <c r="O50" s="43"/>
-      <c r="P50" s="43"/>
-      <c r="Q50" s="43"/>
-      <c r="R50" s="43"/>
-      <c r="S50" s="43"/>
-      <c r="T50" s="43"/>
-      <c r="U50" s="43"/>
-      <c r="V50" s="43"/>
-      <c r="W50" s="43"/>
-      <c r="X50" s="43"/>
-      <c r="Y50" s="43"/>
-      <c r="Z50" s="43"/>
-      <c r="AA50" s="43"/>
-    </row>
-    <row r="51" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="43" t="s">
+    </row>
+    <row r="51" spans="1:7" ht="42" thickBot="1">
+      <c r="A51" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="46" t="s">
+      <c r="C51" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="D51" s="47" t="s">
+      <c r="D51" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E51" s="45" t="s">
+      <c r="E51" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="43"/>
-      <c r="M51" s="43"/>
-      <c r="N51" s="43"/>
-      <c r="O51" s="43"/>
-      <c r="P51" s="43"/>
-      <c r="Q51" s="43"/>
-      <c r="R51" s="43"/>
-      <c r="S51" s="43"/>
-      <c r="T51" s="43"/>
-      <c r="U51" s="43"/>
-      <c r="V51" s="43"/>
-      <c r="W51" s="43"/>
-      <c r="X51" s="43"/>
-      <c r="Y51" s="43"/>
-      <c r="Z51" s="43"/>
-      <c r="AA51" s="43"/>
-    </row>
-    <row r="52" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="49" t="s">
+    </row>
+    <row r="52" spans="1:7" ht="42" thickBot="1">
+      <c r="A52" t="s">
         <v>139</v>
       </c>
-      <c r="B52" s="52" t="s">
+      <c r="B52" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C52" s="52" t="s">
+      <c r="C52" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D52" s="53" t="s">
+      <c r="D52" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="E52" s="50" t="s">
+      <c r="E52" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F52" s="49"/>
-      <c r="G52" s="49"/>
-      <c r="H52" s="49"/>
-      <c r="I52" s="49"/>
-      <c r="J52" s="49"/>
-      <c r="K52" s="49"/>
-      <c r="L52" s="49"/>
-      <c r="M52" s="49"/>
-      <c r="N52" s="49"/>
-      <c r="O52" s="49"/>
-      <c r="P52" s="49"/>
-      <c r="Q52" s="49"/>
-      <c r="R52" s="49"/>
-      <c r="S52" s="49"/>
-      <c r="T52" s="49"/>
-      <c r="U52" s="49"/>
-      <c r="V52" s="49"/>
-      <c r="W52" s="49"/>
-      <c r="X52" s="49"/>
-      <c r="Y52" s="49"/>
-      <c r="Z52" s="49"/>
-      <c r="AA52" s="49"/>
-    </row>
-    <row r="53" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="49" t="s">
+    </row>
+    <row r="53" spans="1:7" ht="42" thickBot="1">
+      <c r="A53" t="s">
         <v>139</v>
       </c>
-      <c r="B53" s="52" t="s">
+      <c r="B53" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C53" s="52" t="s">
+      <c r="C53" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D53" s="53" t="s">
+      <c r="D53" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E53" s="50" t="s">
+      <c r="E53" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="49"/>
-      <c r="I53" s="49"/>
-      <c r="J53" s="49"/>
-      <c r="K53" s="49"/>
-      <c r="L53" s="49"/>
-      <c r="M53" s="49"/>
-      <c r="N53" s="49"/>
-      <c r="O53" s="49"/>
-      <c r="P53" s="49"/>
-      <c r="Q53" s="49"/>
-      <c r="R53" s="49"/>
-      <c r="S53" s="49"/>
-      <c r="T53" s="49"/>
-      <c r="U53" s="49"/>
-      <c r="V53" s="49"/>
-      <c r="W53" s="49"/>
-      <c r="X53" s="49"/>
-      <c r="Y53" s="49"/>
-      <c r="Z53" s="49"/>
-      <c r="AA53" s="49"/>
-    </row>
-    <row r="54" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="49" t="s">
+    </row>
+    <row r="54" spans="1:7" ht="42" thickBot="1">
+      <c r="A54" t="s">
         <v>139</v>
       </c>
-      <c r="B54" s="52" t="s">
+      <c r="B54" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="52" t="s">
+      <c r="C54" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="D54" s="53" t="s">
+      <c r="D54" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="50" t="s">
+      <c r="E54" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="49"/>
-      <c r="J54" s="49"/>
-      <c r="K54" s="49"/>
-      <c r="L54" s="49"/>
-      <c r="M54" s="49"/>
-      <c r="N54" s="49"/>
-      <c r="O54" s="49"/>
-      <c r="P54" s="49"/>
-      <c r="Q54" s="49"/>
-      <c r="R54" s="49"/>
-      <c r="S54" s="49"/>
-      <c r="T54" s="49"/>
-      <c r="U54" s="49"/>
-      <c r="V54" s="49"/>
-      <c r="W54" s="49"/>
-      <c r="X54" s="49"/>
-      <c r="Y54" s="49"/>
-      <c r="Z54" s="49"/>
-      <c r="AA54" s="49"/>
-    </row>
-    <row r="55" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="49" t="s">
+    </row>
+    <row r="55" spans="1:7" ht="42" thickBot="1">
+      <c r="A55" t="s">
         <v>139</v>
       </c>
-      <c r="B55" s="52" t="s">
+      <c r="B55" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="C55" s="52" t="s">
+      <c r="C55" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="D55" s="53" t="s">
+      <c r="D55" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="E55" s="50" t="s">
+      <c r="E55" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="49"/>
-      <c r="I55" s="49"/>
-      <c r="J55" s="49"/>
-      <c r="K55" s="49"/>
-      <c r="L55" s="49"/>
-      <c r="M55" s="49"/>
-      <c r="N55" s="49"/>
-      <c r="O55" s="49"/>
-      <c r="P55" s="49"/>
-      <c r="Q55" s="49"/>
-      <c r="R55" s="49"/>
-      <c r="S55" s="49"/>
-      <c r="T55" s="49"/>
-      <c r="U55" s="49"/>
-      <c r="V55" s="49"/>
-      <c r="W55" s="49"/>
-      <c r="X55" s="49"/>
-      <c r="Y55" s="49"/>
-      <c r="Z55" s="49"/>
-      <c r="AA55" s="49"/>
-    </row>
-    <row r="56" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="49" t="s">
+    </row>
+    <row r="56" spans="1:7" ht="28.2" thickBot="1">
+      <c r="A56" t="s">
         <v>194</v>
       </c>
-      <c r="B56" s="52" t="s">
+      <c r="B56" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="C56" s="52" t="s">
+      <c r="C56" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="D56" s="53" t="s">
+      <c r="D56" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="E56" s="50" t="s">
+      <c r="E56" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-    </row>
-    <row r="57" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="49" t="s">
+    </row>
+    <row r="57" spans="1:7" ht="28.2" thickBot="1">
+      <c r="A57" t="s">
         <v>194</v>
       </c>
-      <c r="B57" s="52" t="s">
+      <c r="B57" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C57" s="52" t="s">
+      <c r="C57" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="D57" s="53" t="s">
+      <c r="D57" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="E57" s="50" t="s">
+      <c r="E57" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-    </row>
-    <row r="58" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="49" t="s">
+    </row>
+    <row r="58" spans="1:7" ht="28.2" thickBot="1">
+      <c r="A58" t="s">
         <v>194</v>
       </c>
-      <c r="B58" s="52" t="s">
+      <c r="B58" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="C58" s="52" t="s">
+      <c r="C58" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="D58" s="53" t="s">
+      <c r="D58" s="14" t="s">
         <v>205</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="F58" s="55"/>
-      <c r="G58" s="56"/>
-    </row>
-    <row r="59" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="49" t="s">
+      <c r="F58" s="17"/>
+      <c r="G58" s="18"/>
+    </row>
+    <row r="59" spans="1:7" ht="28.2" thickBot="1">
+      <c r="A59" t="s">
         <v>194</v>
       </c>
-      <c r="B59" s="52" t="s">
+      <c r="B59" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="C59" s="52" t="s">
+      <c r="C59" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="D59" s="53" t="s">
+      <c r="D59" s="14" t="s">
         <v>209</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="F59" s="54"/>
-      <c r="G59" s="57"/>
-    </row>
-    <row r="60" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="49" t="s">
+      <c r="F59" s="16"/>
+      <c r="G59" s="19"/>
+    </row>
+    <row r="60" spans="1:7" ht="28.2" thickBot="1">
+      <c r="A60" t="s">
         <v>194</v>
       </c>
-      <c r="B60" s="52" t="s">
+      <c r="B60" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="C60" s="52" t="s">
+      <c r="C60" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="D60" s="53" t="s">
+      <c r="D60" s="14" t="s">
         <v>209</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="F60" s="58"/>
-      <c r="G60" s="59"/>
-    </row>
-    <row r="61" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="49" t="s">
+      <c r="F60" s="20"/>
+      <c r="G60" s="21"/>
+    </row>
+    <row r="61" spans="1:7" ht="15" thickBot="1">
+      <c r="A61" t="s">
         <v>214</v>
       </c>
-      <c r="B61" s="52" t="s">
+      <c r="B61" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="C61" s="52" t="s">
+      <c r="C61" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="D61" s="53" t="s">
+      <c r="D61" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="E61" s="50" t="s">
+      <c r="E61" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-    </row>
-    <row r="62" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="49" t="s">
+    </row>
+    <row r="62" spans="1:7" ht="15" thickBot="1">
+      <c r="A62" t="s">
         <v>214</v>
       </c>
-      <c r="B62" s="52" t="s">
+      <c r="B62" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="C62" s="52" t="s">
+      <c r="C62" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D62" s="53" t="s">
+      <c r="D62" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E62" s="50" t="s">
+      <c r="E62" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F62" s="49"/>
-      <c r="G62" s="49"/>
-    </row>
-    <row r="63" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="49" t="s">
+    </row>
+    <row r="63" spans="1:7" ht="15" thickBot="1">
+      <c r="A63" t="s">
         <v>214</v>
       </c>
-      <c r="B63" s="52" t="s">
+      <c r="B63" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="C63" s="52" t="s">
+      <c r="C63" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="D63" s="53" t="s">
+      <c r="D63" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E63" s="50" t="s">
+      <c r="E63" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-    </row>
-    <row r="64" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="49" t="s">
+    </row>
+    <row r="64" spans="1:7" ht="15" thickBot="1">
+      <c r="A64" t="s">
         <v>214</v>
       </c>
-      <c r="B64" s="52" t="s">
+      <c r="B64" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="C64" s="52" t="s">
+      <c r="C64" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="D64" s="53" t="s">
+      <c r="D64" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E64" s="50" t="s">
+      <c r="E64" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-    </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="49" t="s">
+    </row>
+    <row r="65" spans="1:5" ht="15" thickBot="1">
+      <c r="A65" t="s">
         <v>214</v>
       </c>
-      <c r="B65" s="52" t="s">
+      <c r="B65" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="C65" s="52" t="s">
+      <c r="C65" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="D65" s="53" t="s">
+      <c r="D65" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E65" s="50" t="s">
+      <c r="E65" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="F65" s="49"/>
-      <c r="G65" s="49"/>
-    </row>
-    <row r="66" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="49" t="s">
+    </row>
+    <row r="66" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A66" t="s">
         <v>214</v>
       </c>
-      <c r="B66" s="52" t="s">
+      <c r="B66" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="C66" s="52" t="s">
+      <c r="C66" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="D66" s="53" t="s">
+      <c r="D66" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E66" s="50" t="s">
+      <c r="E66" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-    </row>
-    <row r="67" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:5" ht="72">
       <c r="A67" t="s">
         <v>235</v>
       </c>
@@ -3419,12 +3694,12 @@
       <c r="D67" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E67" s="51" t="s">
+      <c r="E67" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="49" t="s">
+    <row r="68" spans="1:5" ht="43.2">
+      <c r="A68" t="s">
         <v>235</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -3436,12 +3711,12 @@
       <c r="D68" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E68" s="50" t="s">
+      <c r="E68" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="49" t="s">
+    <row r="69" spans="1:5" ht="43.2">
+      <c r="A69" t="s">
         <v>235</v>
       </c>
       <c r="B69" s="2" t="s">
@@ -3453,12 +3728,12 @@
       <c r="D69" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E69" s="50" t="s">
+      <c r="E69" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="49" t="s">
+    <row r="70" spans="1:5" ht="57.6">
+      <c r="A70" t="s">
         <v>235</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -3470,12 +3745,12 @@
       <c r="D70" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="E70" s="51" t="s">
+      <c r="E70" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="49" t="s">
+    <row r="71" spans="1:5" ht="43.2">
+      <c r="A71" t="s">
         <v>235</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -3487,11 +3762,11 @@
       <c r="D71" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E71" s="51" t="s">
+      <c r="E71" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="28.8">
       <c r="A72" t="s">
         <v>255</v>
       </c>
@@ -3504,12 +3779,12 @@
       <c r="D72" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="E72" s="51" t="s">
+      <c r="E72" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="49" t="s">
+    <row r="73" spans="1:5" ht="43.2">
+      <c r="A73" t="s">
         <v>255</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -3521,12 +3796,12 @@
       <c r="D73" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="E73" s="51" t="s">
+      <c r="E73" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="49" t="s">
+    <row r="74" spans="1:5" ht="28.8">
+      <c r="A74" t="s">
         <v>255</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -3538,12 +3813,12 @@
       <c r="D74" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="E74" s="51" t="s">
+      <c r="E74" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="49" t="s">
+    <row r="75" spans="1:5" ht="28.8">
+      <c r="A75" t="s">
         <v>255</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -3555,12 +3830,12 @@
       <c r="D75" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="E75" s="51" t="s">
+      <c r="E75" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="49" t="s">
+    <row r="76" spans="1:5" ht="43.2">
+      <c r="A76" t="s">
         <v>255</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -3572,11 +3847,11 @@
       <c r="D76" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E76" s="51" t="s">
+      <c r="E76" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="43.2">
       <c r="A77" t="s">
         <v>270</v>
       </c>
@@ -3589,12 +3864,12 @@
       <c r="D77" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E77" s="51" t="s">
+      <c r="E77" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="49" t="s">
+    <row r="78" spans="1:5" ht="43.2">
+      <c r="A78" t="s">
         <v>270</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -3606,12 +3881,12 @@
       <c r="D78" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E78" s="51" t="s">
+      <c r="E78" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A79" s="49" t="s">
+    <row r="79" spans="1:5" ht="43.2">
+      <c r="A79" t="s">
         <v>270</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -3623,12 +3898,12 @@
       <c r="D79" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E79" s="51" t="s">
+      <c r="E79" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="49" t="s">
+    <row r="80" spans="1:5" ht="57.6">
+      <c r="A80" t="s">
         <v>270</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -3640,12 +3915,12 @@
       <c r="D80" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E80" s="51" t="s">
+      <c r="E80" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="49" t="s">
+    <row r="81" spans="1:5" ht="43.2">
+      <c r="A81" t="s">
         <v>270</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -3657,11 +3932,11 @@
       <c r="D81" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="E81" s="51" t="s">
+      <c r="E81" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="57.6">
       <c r="A82" t="s">
         <v>287</v>
       </c>
@@ -3674,12 +3949,12 @@
       <c r="D82" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E82" s="51" t="s">
+      <c r="E82" s="4" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="49" t="s">
+    <row r="83" spans="1:5" ht="57.6">
+      <c r="A83" t="s">
         <v>287</v>
       </c>
       <c r="B83" s="2" t="s">
@@ -3691,12 +3966,12 @@
       <c r="D83" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E83" s="51" t="s">
+      <c r="E83" s="4" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A84" s="49" t="s">
+    <row r="84" spans="1:5" ht="43.2">
+      <c r="A84" t="s">
         <v>287</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -3708,12 +3983,12 @@
       <c r="D84" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E84" s="51" t="s">
+      <c r="E84" s="4" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="49" t="s">
+    <row r="85" spans="1:5" ht="57.6">
+      <c r="A85" t="s">
         <v>287</v>
       </c>
       <c r="B85" s="2" t="s">
@@ -3725,12 +4000,12 @@
       <c r="D85" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E85" s="51" t="s">
+      <c r="E85" s="4" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="49" t="s">
+    <row r="86" spans="1:5" ht="57.6">
+      <c r="A86" t="s">
         <v>287</v>
       </c>
       <c r="B86" s="2" t="s">
@@ -3742,8 +4017,1128 @@
       <c r="D86" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E86" s="51" t="s">
+      <c r="E86" s="4" t="s">
         <v>307</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="43.2">
+      <c r="A87" t="s">
+        <v>308</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="43.2">
+      <c r="A88" t="s">
+        <v>308</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="43.2">
+      <c r="A89" t="s">
+        <v>308</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="43.2">
+      <c r="A90" t="s">
+        <v>308</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="43.2">
+      <c r="A91" t="s">
+        <v>308</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15" thickBot="1">
+      <c r="A92" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B92" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="C92" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D92" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E92" s="24" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15" thickBot="1">
+      <c r="A93" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B93" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="C93" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E93" s="24" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15" thickBot="1">
+      <c r="A94" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B94" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="C94" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E94" s="24" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15" thickBot="1">
+      <c r="A95" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B95" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="C95" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="D95" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="E95" s="24" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15" thickBot="1">
+      <c r="A96" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B96" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="C96" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="D96" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E96" s="24" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A97" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B97" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="C97" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="D97" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15" thickBot="1">
+      <c r="A98" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B98" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="C98" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="D98" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E98" s="24" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A99" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B99" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="C99" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="D99" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E99" s="24" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15" thickBot="1">
+      <c r="A100" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B100" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="C100" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="D100" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A101" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B101" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="C101" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="D101" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="E101" s="24" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A102" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B102" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="C102" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="D102" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15" thickBot="1">
+      <c r="A103" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B103" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="C103" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="D103" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="E103" s="24" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A104" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B104" s="26" t="s">
+        <v>370</v>
+      </c>
+      <c r="C104" s="26" t="s">
+        <v>371</v>
+      </c>
+      <c r="D104" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A105" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B105" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="C105" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="D105" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="E105" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A106" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B106" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="C106" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A107" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B107" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="C107" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="D107" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="E107" s="24" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A108" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B108" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="C108" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="D108" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="E108" s="24" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A109" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B109" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="C109" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="D109" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="E109" s="28" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A110" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B110" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="C110" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="D110" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E110" s="24" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A111" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B111" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="D111" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E111" s="24" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A112" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B112" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="C112" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="D112" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E112" s="24" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A113" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B113" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="C113" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="D113" s="27" t="s">
+        <v>402</v>
+      </c>
+      <c r="E113" s="24" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A114" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B114" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="C114" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="D114" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E114" s="24" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15" thickBot="1">
+      <c r="A115" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B115" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="C115" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="D115" s="27" t="s">
+        <v>409</v>
+      </c>
+      <c r="E115" s="24" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A116" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B116" s="26" t="s">
+        <v>411</v>
+      </c>
+      <c r="C116" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="D116" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E116" s="24" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A117" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B117" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="C117" s="26" t="s">
+        <v>415</v>
+      </c>
+      <c r="D117" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E117" s="24" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="15" thickBot="1">
+      <c r="A118" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B118" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="C118" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="D118" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="E118" s="24" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A119" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B119" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="C119" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="D119" s="27" t="s">
+        <v>422</v>
+      </c>
+      <c r="E119" s="24" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15" thickBot="1">
+      <c r="A120" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B120" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="C120" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="D120" s="27" t="s">
+        <v>426</v>
+      </c>
+      <c r="E120" s="24" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A121" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B121" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="C121" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="D121" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E121" s="24" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A122" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B122" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="C122" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="D122" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E122" s="24" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A123" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B123" s="26" t="s">
+        <v>434</v>
+      </c>
+      <c r="C123" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="D123" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E123" s="24" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A124" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B124" s="26" t="s">
+        <v>437</v>
+      </c>
+      <c r="C124" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="D124" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="E124" s="24" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A125" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B125" s="26" t="s">
+        <v>440</v>
+      </c>
+      <c r="C125" s="26" t="s">
+        <v>441</v>
+      </c>
+      <c r="D125" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E125" s="24" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="42" thickBot="1">
+      <c r="A126" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="B126" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="C126" s="26" t="s">
+        <v>444</v>
+      </c>
+      <c r="D126" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="E126" s="24" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="42" thickBot="1">
+      <c r="A127" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B127" s="26" t="s">
+        <v>447</v>
+      </c>
+      <c r="C127" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="D127" s="27" t="s">
+        <v>449</v>
+      </c>
+      <c r="E127" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="55.8" thickBot="1">
+      <c r="A128" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B128" s="26" t="s">
+        <v>451</v>
+      </c>
+      <c r="C128" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="D128" s="27" t="s">
+        <v>453</v>
+      </c>
+      <c r="E128" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="42" thickBot="1">
+      <c r="A129" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B129" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="C129" s="26" t="s">
+        <v>455</v>
+      </c>
+      <c r="D129" s="27" t="s">
+        <v>456</v>
+      </c>
+      <c r="E129" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15" thickBot="1">
+      <c r="A130" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B130" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="C130" s="26" t="s">
+        <v>458</v>
+      </c>
+      <c r="D130" s="27" t="s">
+        <v>458</v>
+      </c>
+      <c r="E130" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15" thickBot="1">
+      <c r="A131" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B131" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="C131" s="26" t="s">
+        <v>458</v>
+      </c>
+      <c r="D131" s="27" t="s">
+        <v>458</v>
+      </c>
+      <c r="E131" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="42" thickBot="1">
+      <c r="A132" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B132" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="C132" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="D132" s="27" t="s">
+        <v>462</v>
+      </c>
+      <c r="E132" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="42" thickBot="1">
+      <c r="A133" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B133" s="26" t="s">
+        <v>463</v>
+      </c>
+      <c r="C133" s="26" t="s">
+        <v>464</v>
+      </c>
+      <c r="D133" s="27" t="s">
+        <v>456</v>
+      </c>
+      <c r="E133" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="42" thickBot="1">
+      <c r="A134" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B134" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="C134" s="26" t="s">
+        <v>466</v>
+      </c>
+      <c r="D134" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="E134" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="42" thickBot="1">
+      <c r="A135" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B135" s="26" t="s">
+        <v>468</v>
+      </c>
+      <c r="C135" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="D135" s="27" t="s">
+        <v>456</v>
+      </c>
+      <c r="E135" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="42" thickBot="1">
+      <c r="A136" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B136" s="26" t="s">
+        <v>470</v>
+      </c>
+      <c r="C136" s="26" t="s">
+        <v>471</v>
+      </c>
+      <c r="D136" s="27" t="s">
+        <v>472</v>
+      </c>
+      <c r="E136" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="28.2" thickBot="1">
+      <c r="A137" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B137" s="26" t="s">
+        <v>473</v>
+      </c>
+      <c r="C137" s="26" t="s">
+        <v>474</v>
+      </c>
+      <c r="D137" s="27" t="s">
+        <v>456</v>
+      </c>
+      <c r="E137" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="43.2">
+      <c r="A138" s="24" t="s">
+        <v>475</v>
+      </c>
+      <c r="B138" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="C138" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E138" s="28" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="43.2">
+      <c r="A139" s="24" t="s">
+        <v>475</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="E139" s="28" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="57.6">
+      <c r="A140" s="24" t="s">
+        <v>475</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="43.2">
+      <c r="A141" s="24" t="s">
+        <v>475</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="43.2">
+      <c r="A142" s="24" t="s">
+        <v>475</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="57.6">
+      <c r="A143" t="s">
+        <v>494</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="86.4">
+      <c r="A144" s="24" t="s">
+        <v>494</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="E144" s="4" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="57.6">
+      <c r="A145" s="24" t="s">
+        <v>494</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="72">
+      <c r="A146" s="24" t="s">
+        <v>494</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="E146" s="28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="72">
+      <c r="A147" s="24" t="s">
+        <v>494</v>
+      </c>
+      <c r="B147" s="24"/>
+      <c r="C147" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="57.6">
+      <c r="A148" t="s">
+        <v>509</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="E148" s="4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="43.2">
+      <c r="A149" s="24" t="s">
+        <v>509</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="43.2">
+      <c r="A150" s="24" t="s">
+        <v>509</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="43.2">
+      <c r="A151" s="24" t="s">
+        <v>509</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="43.2">
+      <c r="A152" s="24" t="s">
+        <v>509</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -3833,9 +5228,41 @@
     <hyperlink ref="E46" r:id="rId83" xr:uid="{CB9AFBD2-2016-47F4-A101-FC61F822B036}"/>
     <hyperlink ref="E49" r:id="rId84" xr:uid="{FA3D8241-3756-4DA1-87E7-C74699704A80}"/>
     <hyperlink ref="E50" r:id="rId85" xr:uid="{DD7B1248-6D8C-4877-B4D4-904219781023}"/>
+    <hyperlink ref="E87" r:id="rId86" xr:uid="{8A5ADE8E-C1C5-4E21-BC22-FE1F729F5B2B}"/>
+    <hyperlink ref="E88" r:id="rId87" xr:uid="{EAB833AE-16BA-4792-BECC-2A0F4A662C90}"/>
+    <hyperlink ref="E89" r:id="rId88" xr:uid="{08D6AC4F-BF42-47EA-AA17-EAE6086C855B}"/>
+    <hyperlink ref="E90" r:id="rId89" xr:uid="{562715D9-BD20-41E1-9BB8-849502FA6F9D}"/>
+    <hyperlink ref="E91" r:id="rId90" xr:uid="{89989E8C-F1BC-4690-AB9F-EEDD3B6AF31D}"/>
+    <hyperlink ref="E109" r:id="rId91" xr:uid="{8C81FFCE-973A-42B9-BF21-455C55BAA068}"/>
+    <hyperlink ref="E130" r:id="rId92" xr:uid="{CD6CD1AE-2702-4C43-89FE-272C0B6706AD}"/>
+    <hyperlink ref="E137" r:id="rId93" xr:uid="{D3D601FB-5649-4C52-8005-ADCC9D2EDF43}"/>
+    <hyperlink ref="E136" r:id="rId94" xr:uid="{1FCF3137-047F-4841-B5A1-7650E89E4F5E}"/>
+    <hyperlink ref="E135" r:id="rId95" xr:uid="{26C82423-BAE7-44D7-8509-C39DB36473A4}"/>
+    <hyperlink ref="E134" r:id="rId96" xr:uid="{1396C837-F04E-439C-8F2B-A6586272897C}"/>
+    <hyperlink ref="E133" r:id="rId97" xr:uid="{3D244E90-4CA9-45EA-B454-167B07C47D85}"/>
+    <hyperlink ref="E132" r:id="rId98" xr:uid="{76C3FF1A-E5B4-424D-A3E0-4F3AACDB641E}"/>
+    <hyperlink ref="E131" r:id="rId99" xr:uid="{89F5EEA8-56CE-4632-871E-D4954B50222F}"/>
+    <hyperlink ref="E129" r:id="rId100" xr:uid="{D6FD9532-5EF1-4B53-BC2A-D3A49FF9C900}"/>
+    <hyperlink ref="E128" r:id="rId101" xr:uid="{766095ED-4DAA-43A7-A7B9-5A939FC75740}"/>
+    <hyperlink ref="E127" r:id="rId102" xr:uid="{46993E1C-68EA-45EA-8D15-4BB284D01192}"/>
+    <hyperlink ref="E138" r:id="rId103" xr:uid="{4AE74D90-BE59-45D6-9EBE-B7EB922F207B}"/>
+    <hyperlink ref="E139" r:id="rId104" xr:uid="{D4DDF3C4-354D-4847-A9F6-DDBAEFBC80EC}"/>
+    <hyperlink ref="E140" r:id="rId105" xr:uid="{01A3BCE9-508D-47B5-BAE2-6A97A837124A}"/>
+    <hyperlink ref="E141" r:id="rId106" xr:uid="{954BFEE1-5726-4627-8950-97B05BE311F9}"/>
+    <hyperlink ref="E142" r:id="rId107" xr:uid="{E375A123-0CEB-4571-8BE0-AF0D6FA2272C}"/>
+    <hyperlink ref="E143" r:id="rId108" xr:uid="{F30A3C74-7CBD-41F0-B13B-C5D2E2863D4B}"/>
+    <hyperlink ref="E144" r:id="rId109" xr:uid="{8DCEF8B3-753D-4EB2-9E52-BC8D9D62E06F}"/>
+    <hyperlink ref="E145" r:id="rId110" xr:uid="{7D14D789-72C2-41FE-A0D5-323743513E5B}"/>
+    <hyperlink ref="E146" r:id="rId111" xr:uid="{231EEF9B-04FB-40D3-B3CA-E1E9600663EC}"/>
+    <hyperlink ref="E147" r:id="rId112" xr:uid="{EC544ACC-F7B3-4C7F-A35C-50E6C3D2282A}"/>
+    <hyperlink ref="E148" r:id="rId113" xr:uid="{6749BAA6-059C-4438-8655-E03F2B4D8891}"/>
+    <hyperlink ref="E149" r:id="rId114" location="gsc.tab=0" xr:uid="{A1FDDDBB-95C3-4A4B-9C24-0F4F1DC874AF}"/>
+    <hyperlink ref="E150" r:id="rId115" xr:uid="{0D9A781A-A28D-470A-B332-8F20939D4523}"/>
+    <hyperlink ref="E151" r:id="rId116" xr:uid="{5A0492E4-FC92-4460-9542-4522A73A9702}"/>
+    <hyperlink ref="E152" r:id="rId117" xr:uid="{14C80455-9561-4D9D-9AA3-4C7A714C710B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId86"/>
+  <pageSetup orientation="portrait" r:id="rId118"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">

</xml_diff>